<commit_message>
Correçao da planilha do demonstrativo financeiro.
</commit_message>
<xml_diff>
--- a/sme_ptrf_apps/static/cargas/modelo_demonstrativo_financeiro.xlsx
+++ b/sme_ptrf_apps/static/cargas/modelo_demonstrativo_financeiro.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="63">
   <si>
     <t xml:space="preserve">Prefeitura do Município de São Paulo</t>
   </si>
@@ -41,9 +41,6 @@
     <t xml:space="preserve">01 - Período de realização</t>
   </si>
   <si>
-    <t xml:space="preserve">[Preenchimento sistema - prestação de contas]</t>
-  </si>
-  <si>
     <t xml:space="preserve">02 - Ação</t>
   </si>
   <si>
@@ -65,9 +62,6 @@
     <t xml:space="preserve">07 - Diretoria Regional de Educação</t>
   </si>
   <si>
-    <t xml:space="preserve">[Preenchimento sistema - dados Associação]</t>
-  </si>
-  <si>
     <t xml:space="preserve">BLOCO 2 - SÍNTESE DA RECEITA E DA DESPESA (R$)</t>
   </si>
   <si>
@@ -95,318 +89,6 @@
     <t xml:space="preserve">15 - Total reprogramado</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">C </t>
-    </r>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">[Preenchimento sistema - reprogramado]</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">C </t>
-    </r>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">[Preenchimento sistema - carga inicial]</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">C </t>
-    </r>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">[Preenchimento sistema - cadastro receita] - Apenas para o PTRF Básico</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">C </t>
-    </r>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">[Preenchimento sistema  - cadastro de receita]</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">C</t>
-    </r>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> [Cálculo 08+09+10+11]</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">C </t>
-    </r>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">[Preenchimento sistema - cadastro despesa custeio]</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">C </t>
-    </r>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">[Cálculo 12-13]</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">[Soma 14 C+K]</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">K </t>
-    </r>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">[Preenchimento sistema - reprogramado]</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">K </t>
-    </r>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">[Preenchimento sistema - carga inicial]</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">K </t>
-    </r>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">[Preenchimento sistema  - cadastro de receita]</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">K </t>
-    </r>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">[Cálculo 08+09+11]</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">K </t>
-    </r>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">[Preenchimento sistema - cadastro despesa capital]</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">K</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">[Cálculo 12-13]</t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve">BLOCO 3 - PAGAMENTOS EFETUADOS E DEMONSTRADOS</t>
   </si>
   <si>
@@ -452,9 +134,6 @@
     <t xml:space="preserve">26 - Valor</t>
   </si>
   <si>
-    <t xml:space="preserve">No caso do cheque, na opção, deve-se apresentar o número.</t>
-  </si>
-  <si>
     <t xml:space="preserve">BLOCO 4 - DÉBITOS NÃO DEMONSTRADOS NO EXTRATO DO PERÍODO</t>
   </si>
   <si>
@@ -509,22 +188,7 @@
     <t xml:space="preserve">41 - Valor </t>
   </si>
   <si>
-    <t xml:space="preserve">[Numerar os itens. Ordená-los ordem crescente de data do documento]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[Preenchimento sistema - cadastro receita]</t>
-  </si>
-  <si>
     <t xml:space="preserve">BLOCO 6 - OBSERVAÇÃO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[Campo aberto para preenchimento da APM, para duas situações em especial:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Divergências nas datas ou valores constantes nos documentos apresentados no Bloco 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Devolução de recursos - irregularidades]</t>
   </si>
   <si>
     <t xml:space="preserve">BLOCO 7 - ASSINATURA DOS RESPONSÁVEIS PELA PRESTAÇÃO DE CONTAS</t>
@@ -669,7 +333,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <i val="true"/>
       <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -685,6 +348,7 @@
       <charset val="1"/>
     </font>
     <font>
+      <i val="true"/>
       <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -740,14 +404,14 @@
       <left style="thin"/>
       <right style="thin"/>
       <top style="thin"/>
-      <bottom style="thin"/>
+      <bottom/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
       <left style="thin"/>
       <right style="thin"/>
       <top style="thin"/>
-      <bottom/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -848,7 +512,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="66">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -881,23 +545,23 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="15" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -909,7 +573,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -941,11 +605,11 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -953,31 +617,31 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -985,35 +649,31 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
@@ -1061,15 +721,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1089,32 +741,36 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1209,9 +865,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>60480</xdr:colOff>
+      <xdr:colOff>59400</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>130680</xdr:rowOff>
+      <xdr:rowOff>129600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1225,7 +881,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="66600" y="152280"/>
-          <a:ext cx="640800" cy="540360"/>
+          <a:ext cx="639720" cy="539280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1247,8 +903,8 @@
   </sheetPr>
   <dimension ref="A2:Y1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A23" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1305,34 +961,28 @@
         <v>5</v>
       </c>
       <c r="I5" s="8"/>
-      <c r="J5" s="9" t="s">
-        <v>6</v>
-      </c>
+      <c r="J5" s="9"/>
       <c r="K5" s="9"/>
     </row>
     <row r="6" s="7" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="H6" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I6" s="8"/>
-      <c r="J6" s="10" t="s">
-        <v>6</v>
-      </c>
+      <c r="J6" s="10"/>
       <c r="K6" s="10"/>
     </row>
     <row r="7" s="7" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="H7" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I7" s="8"/>
-      <c r="J7" s="11" t="s">
-        <v>6</v>
-      </c>
+      <c r="J7" s="11"/>
       <c r="K7" s="11"/>
     </row>
     <row r="9" s="7" customFormat="true" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="12"/>
       <c r="C9" s="12"/>
@@ -1347,7 +997,7 @@
     </row>
     <row r="10" s="7" customFormat="true" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" s="13"/>
       <c r="C10" s="13"/>
@@ -1355,36 +1005,28 @@
       <c r="E10" s="13"/>
       <c r="F10" s="13"/>
       <c r="G10" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="H10" s="14" t="s">
+      <c r="I10" s="15" t="s">
         <v>12</v>
-      </c>
-      <c r="I10" s="15" t="s">
-        <v>13</v>
       </c>
       <c r="J10" s="15"/>
       <c r="K10" s="15"/>
       <c r="P10" s="16"/>
     </row>
     <row r="11" s="20" customFormat="true" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="17" t="s">
-        <v>14</v>
-      </c>
+      <c r="A11" s="17"/>
       <c r="B11" s="17"/>
       <c r="C11" s="17"/>
       <c r="D11" s="17"/>
       <c r="E11" s="17"/>
       <c r="F11" s="17"/>
-      <c r="G11" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="H11" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="I11" s="19" t="s">
-        <v>14</v>
-      </c>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="19"/>
       <c r="J11" s="19"/>
       <c r="K11" s="19"/>
     </row>
@@ -1402,7 +1044,7 @@
     </row>
     <row r="13" s="7" customFormat="true" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="12" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B13" s="12"/>
       <c r="C13" s="12"/>
@@ -1417,91 +1059,63 @@
     </row>
     <row r="14" s="7" customFormat="true" ht="32.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="24" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B14" s="24"/>
       <c r="C14" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" s="27" t="s">
         <v>17</v>
-      </c>
-      <c r="D14" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="E14" s="27" t="s">
-        <v>19</v>
       </c>
       <c r="F14" s="27"/>
       <c r="G14" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="H14" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="I14" s="27" t="s">
         <v>20</v>
-      </c>
-      <c r="H14" s="26" t="s">
-        <v>21</v>
-      </c>
-      <c r="I14" s="27" t="s">
-        <v>22</v>
       </c>
       <c r="J14" s="27"/>
       <c r="K14" s="26" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" s="7" customFormat="true" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="29" t="s">
-        <v>24</v>
-      </c>
+      <c r="A15" s="29"/>
       <c r="B15" s="29"/>
-      <c r="C15" s="30" t="s">
-        <v>25</v>
-      </c>
-      <c r="D15" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="E15" s="29" t="s">
-        <v>27</v>
-      </c>
+      <c r="C15" s="30"/>
+      <c r="D15" s="29"/>
+      <c r="E15" s="29"/>
       <c r="F15" s="29"/>
-      <c r="G15" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="H15" s="31" t="s">
-        <v>29</v>
-      </c>
-      <c r="I15" s="32" t="s">
-        <v>30</v>
-      </c>
+      <c r="G15" s="31"/>
+      <c r="H15" s="31"/>
+      <c r="I15" s="32"/>
       <c r="J15" s="32"/>
-      <c r="K15" s="33" t="s">
-        <v>31</v>
-      </c>
+      <c r="K15" s="33"/>
     </row>
     <row r="16" s="7" customFormat="true" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="34" t="s">
-        <v>32</v>
-      </c>
+      <c r="A16" s="34"/>
       <c r="B16" s="34"/>
-      <c r="C16" s="35" t="s">
-        <v>33</v>
-      </c>
+      <c r="C16" s="35"/>
       <c r="D16" s="36"/>
-      <c r="E16" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="F16" s="34"/>
-      <c r="G16" s="37" t="s">
-        <v>35</v>
-      </c>
-      <c r="H16" s="38" t="s">
-        <v>36</v>
-      </c>
-      <c r="I16" s="39" t="s">
-        <v>37</v>
-      </c>
-      <c r="J16" s="39"/>
+      <c r="E16" s="37"/>
+      <c r="F16" s="37"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="18"/>
+      <c r="I16" s="33"/>
+      <c r="J16" s="33"/>
       <c r="K16" s="33"/>
     </row>
     <row r="17" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="18" s="40" customFormat="true" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="18" s="39" customFormat="true" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="12" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="12"/>
@@ -1514,103 +1128,101 @@
       <c r="J18" s="12"/>
       <c r="K18" s="12"/>
     </row>
-    <row r="19" s="43" customFormat="true" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="41" t="s">
-        <v>39</v>
-      </c>
-      <c r="B19" s="42" t="s">
-        <v>40</v>
-      </c>
-      <c r="C19" s="42"/>
-      <c r="D19" s="42"/>
-      <c r="E19" s="42"/>
-      <c r="F19" s="42"/>
-      <c r="G19" s="43" t="s">
-        <v>41</v>
-      </c>
-      <c r="I19" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="J19" s="42"/>
-      <c r="K19" s="42"/>
-    </row>
-    <row r="20" s="51" customFormat="true" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="41"/>
-      <c r="B20" s="44" t="s">
-        <v>43</v>
-      </c>
-      <c r="C20" s="45" t="s">
-        <v>44</v>
-      </c>
-      <c r="D20" s="45" t="s">
-        <v>45</v>
-      </c>
-      <c r="E20" s="46" t="s">
-        <v>46</v>
-      </c>
-      <c r="F20" s="47" t="s">
-        <v>47</v>
-      </c>
-      <c r="G20" s="45" t="s">
-        <v>48</v>
-      </c>
-      <c r="H20" s="45" t="s">
-        <v>49</v>
-      </c>
-      <c r="I20" s="48" t="s">
-        <v>50</v>
-      </c>
-      <c r="J20" s="46" t="s">
-        <v>51</v>
-      </c>
-      <c r="K20" s="49" t="s">
-        <v>52</v>
-      </c>
-      <c r="L20" s="50"/>
-      <c r="N20" s="52"/>
-      <c r="O20" s="52"/>
-      <c r="Q20" s="52"/>
-      <c r="R20" s="52"/>
-      <c r="S20" s="50"/>
-      <c r="U20" s="50"/>
-      <c r="V20" s="50"/>
-      <c r="W20" s="50"/>
-      <c r="X20" s="50"/>
-      <c r="Y20" s="50"/>
-    </row>
-    <row r="21" s="56" customFormat="true" ht="56.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="39" t="n">
+    <row r="19" s="42" customFormat="true" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" s="41"/>
+      <c r="D19" s="41"/>
+      <c r="E19" s="41"/>
+      <c r="F19" s="41"/>
+      <c r="G19" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="I19" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="J19" s="41"/>
+      <c r="K19" s="41"/>
+    </row>
+    <row r="20" s="50" customFormat="true" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="40"/>
+      <c r="B20" s="43" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="44" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" s="44" t="s">
+        <v>29</v>
+      </c>
+      <c r="E20" s="45" t="s">
+        <v>30</v>
+      </c>
+      <c r="F20" s="46" t="s">
+        <v>31</v>
+      </c>
+      <c r="G20" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="H20" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="I20" s="47" t="s">
+        <v>34</v>
+      </c>
+      <c r="J20" s="45" t="s">
+        <v>35</v>
+      </c>
+      <c r="K20" s="48" t="s">
+        <v>36</v>
+      </c>
+      <c r="L20" s="49"/>
+      <c r="N20" s="51"/>
+      <c r="O20" s="51"/>
+      <c r="Q20" s="51"/>
+      <c r="R20" s="51"/>
+      <c r="S20" s="49"/>
+      <c r="U20" s="49"/>
+      <c r="V20" s="49"/>
+      <c r="W20" s="49"/>
+      <c r="X20" s="49"/>
+      <c r="Y20" s="49"/>
+    </row>
+    <row r="21" s="53" customFormat="true" ht="56.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="33" t="n">
         <v>1</v>
       </c>
-      <c r="B21" s="53"/>
-      <c r="C21" s="37"/>
-      <c r="D21" s="54"/>
-      <c r="E21" s="54"/>
-      <c r="F21" s="54"/>
-      <c r="G21" s="55"/>
-      <c r="H21" s="54"/>
-      <c r="I21" s="18" t="s">
-        <v>53</v>
-      </c>
+      <c r="B21" s="18"/>
+      <c r="C21" s="38"/>
+      <c r="D21" s="38"/>
+      <c r="E21" s="38"/>
+      <c r="F21" s="38"/>
+      <c r="G21" s="52"/>
+      <c r="H21" s="38"/>
+      <c r="I21" s="18"/>
       <c r="J21" s="18"/>
       <c r="K21" s="18"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="57"/>
-      <c r="B22" s="56"/>
-      <c r="C22" s="56"/>
-      <c r="D22" s="56"/>
-      <c r="E22" s="56"/>
-      <c r="F22" s="56"/>
-      <c r="G22" s="56"/>
-      <c r="H22" s="56"/>
-      <c r="I22" s="56"/>
-      <c r="J22" s="56"/>
-      <c r="K22" s="56"/>
-    </row>
-    <row r="23" s="40" customFormat="true" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="54"/>
+      <c r="B22" s="53"/>
+      <c r="C22" s="53"/>
+      <c r="D22" s="53"/>
+      <c r="E22" s="53"/>
+      <c r="F22" s="53"/>
+      <c r="G22" s="53"/>
+      <c r="H22" s="53"/>
+      <c r="I22" s="53"/>
+      <c r="J22" s="53"/>
+      <c r="K22" s="53"/>
+    </row>
+    <row r="23" s="39" customFormat="true" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="12" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="B23" s="12"/>
       <c r="C23" s="12"/>
@@ -1623,72 +1235,72 @@
       <c r="J23" s="12"/>
       <c r="K23" s="12"/>
     </row>
-    <row r="24" s="43" customFormat="true" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="41" t="s">
-        <v>55</v>
-      </c>
-      <c r="B24" s="42" t="s">
+    <row r="24" s="42" customFormat="true" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="40" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" s="41"/>
+      <c r="D24" s="41"/>
+      <c r="E24" s="41"/>
+      <c r="F24" s="41"/>
+      <c r="G24" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="I24" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="J24" s="41"/>
+      <c r="K24" s="41"/>
+    </row>
+    <row r="25" s="50" customFormat="true" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="40"/>
+      <c r="B25" s="43" t="s">
         <v>40</v>
       </c>
-      <c r="C24" s="42"/>
-      <c r="D24" s="42"/>
-      <c r="E24" s="42"/>
-      <c r="F24" s="42"/>
-      <c r="G24" s="43" t="s">
+      <c r="C25" s="44" t="s">
         <v>41</v>
       </c>
-      <c r="I24" s="42" t="s">
-        <v>56</v>
-      </c>
-      <c r="J24" s="42"/>
-      <c r="K24" s="42"/>
-    </row>
-    <row r="25" s="51" customFormat="true" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="41"/>
-      <c r="B25" s="44" t="s">
-        <v>57</v>
-      </c>
-      <c r="C25" s="45" t="s">
-        <v>58</v>
-      </c>
-      <c r="D25" s="45" t="s">
-        <v>59</v>
-      </c>
-      <c r="E25" s="46" t="s">
-        <v>60</v>
-      </c>
-      <c r="F25" s="47" t="s">
-        <v>61</v>
-      </c>
-      <c r="G25" s="45" t="s">
-        <v>62</v>
-      </c>
-      <c r="H25" s="45" t="s">
-        <v>63</v>
-      </c>
-      <c r="I25" s="48" t="s">
-        <v>64</v>
-      </c>
-      <c r="J25" s="46" t="s">
-        <v>65</v>
-      </c>
-      <c r="K25" s="49" t="s">
-        <v>66</v>
-      </c>
-      <c r="L25" s="50"/>
-      <c r="N25" s="52"/>
-      <c r="O25" s="52"/>
-      <c r="Q25" s="52"/>
-      <c r="R25" s="52"/>
-      <c r="S25" s="50"/>
-      <c r="U25" s="50"/>
-      <c r="V25" s="50"/>
-      <c r="W25" s="50"/>
-      <c r="X25" s="50"/>
-      <c r="Y25" s="50"/>
-    </row>
-    <row r="26" s="59" customFormat="true" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="58"/>
+      <c r="D25" s="44" t="s">
+        <v>42</v>
+      </c>
+      <c r="E25" s="45" t="s">
+        <v>43</v>
+      </c>
+      <c r="F25" s="46" t="s">
+        <v>44</v>
+      </c>
+      <c r="G25" s="44" t="s">
+        <v>45</v>
+      </c>
+      <c r="H25" s="44" t="s">
+        <v>46</v>
+      </c>
+      <c r="I25" s="47" t="s">
+        <v>47</v>
+      </c>
+      <c r="J25" s="45" t="s">
+        <v>48</v>
+      </c>
+      <c r="K25" s="48" t="s">
+        <v>49</v>
+      </c>
+      <c r="L25" s="49"/>
+      <c r="N25" s="51"/>
+      <c r="O25" s="51"/>
+      <c r="Q25" s="51"/>
+      <c r="R25" s="51"/>
+      <c r="S25" s="49"/>
+      <c r="U25" s="49"/>
+      <c r="V25" s="49"/>
+      <c r="W25" s="49"/>
+      <c r="X25" s="49"/>
+      <c r="Y25" s="49"/>
+    </row>
+    <row r="26" s="56" customFormat="true" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="55"/>
       <c r="B26" s="18"/>
       <c r="C26" s="18"/>
       <c r="D26" s="18"/>
@@ -1701,21 +1313,21 @@
       <c r="K26" s="18"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="57"/>
-      <c r="B27" s="56"/>
-      <c r="C27" s="56"/>
-      <c r="D27" s="56"/>
-      <c r="E27" s="56"/>
-      <c r="F27" s="56"/>
-      <c r="G27" s="56"/>
-      <c r="H27" s="56"/>
-      <c r="I27" s="56"/>
-      <c r="J27" s="56"/>
-      <c r="K27" s="56"/>
+      <c r="A27" s="54"/>
+      <c r="B27" s="53"/>
+      <c r="C27" s="53"/>
+      <c r="D27" s="53"/>
+      <c r="E27" s="53"/>
+      <c r="F27" s="53"/>
+      <c r="G27" s="53"/>
+      <c r="H27" s="53"/>
+      <c r="I27" s="53"/>
+      <c r="J27" s="53"/>
+      <c r="K27" s="53"/>
     </row>
     <row r="28" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="12" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="B28" s="12"/>
       <c r="C28" s="12"/>
@@ -1729,63 +1341,55 @@
       <c r="K28" s="12"/>
     </row>
     <row r="29" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="60" t="s">
-        <v>68</v>
-      </c>
-      <c r="B29" s="61" t="s">
-        <v>69</v>
-      </c>
-      <c r="C29" s="61"/>
-      <c r="D29" s="61"/>
-      <c r="E29" s="61"/>
-      <c r="F29" s="61" t="s">
-        <v>70</v>
-      </c>
-      <c r="G29" s="61"/>
-      <c r="H29" s="61" t="s">
-        <v>71</v>
-      </c>
-      <c r="I29" s="61"/>
-      <c r="J29" s="61"/>
-      <c r="K29" s="61"/>
+      <c r="A29" s="57" t="s">
+        <v>51</v>
+      </c>
+      <c r="B29" s="58" t="s">
+        <v>52</v>
+      </c>
+      <c r="C29" s="58"/>
+      <c r="D29" s="58"/>
+      <c r="E29" s="58"/>
+      <c r="F29" s="58" t="s">
+        <v>53</v>
+      </c>
+      <c r="G29" s="58"/>
+      <c r="H29" s="58" t="s">
+        <v>54</v>
+      </c>
+      <c r="I29" s="58"/>
+      <c r="J29" s="58"/>
+      <c r="K29" s="58"/>
     </row>
     <row r="30" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="62" t="s">
-        <v>72</v>
-      </c>
-      <c r="B30" s="63" t="s">
-        <v>73</v>
-      </c>
-      <c r="C30" s="63"/>
-      <c r="D30" s="63"/>
-      <c r="E30" s="63"/>
-      <c r="F30" s="63" t="s">
-        <v>73</v>
-      </c>
-      <c r="G30" s="63"/>
-      <c r="H30" s="64" t="s">
-        <v>73</v>
-      </c>
-      <c r="I30" s="64"/>
-      <c r="J30" s="64"/>
-      <c r="K30" s="64"/>
+      <c r="A30" s="59"/>
+      <c r="B30" s="60"/>
+      <c r="C30" s="60"/>
+      <c r="D30" s="60"/>
+      <c r="E30" s="60"/>
+      <c r="F30" s="60"/>
+      <c r="G30" s="60"/>
+      <c r="H30" s="61"/>
+      <c r="I30" s="61"/>
+      <c r="J30" s="61"/>
+      <c r="K30" s="61"/>
     </row>
     <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="57"/>
-      <c r="B31" s="56"/>
-      <c r="C31" s="56"/>
-      <c r="D31" s="56"/>
-      <c r="E31" s="56"/>
-      <c r="F31" s="56"/>
-      <c r="G31" s="56"/>
-      <c r="H31" s="56"/>
-      <c r="I31" s="56"/>
-      <c r="J31" s="56"/>
-      <c r="K31" s="56"/>
+      <c r="A31" s="54"/>
+      <c r="B31" s="53"/>
+      <c r="C31" s="53"/>
+      <c r="D31" s="53"/>
+      <c r="E31" s="53"/>
+      <c r="F31" s="53"/>
+      <c r="G31" s="53"/>
+      <c r="H31" s="53"/>
+      <c r="I31" s="53"/>
+      <c r="J31" s="53"/>
+      <c r="K31" s="53"/>
     </row>
     <row r="32" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="12" t="s">
-        <v>74</v>
+        <v>55</v>
       </c>
       <c r="B32" s="12"/>
       <c r="C32" s="12"/>
@@ -1799,47 +1403,41 @@
       <c r="K32" s="12"/>
     </row>
     <row r="33" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="65" t="s">
-        <v>75</v>
-      </c>
+      <c r="A33" s="62"/>
       <c r="B33" s="16"/>
       <c r="C33" s="16"/>
-      <c r="D33" s="56"/>
-      <c r="E33" s="56"/>
-      <c r="F33" s="56"/>
-      <c r="G33" s="56"/>
-      <c r="H33" s="56"/>
-      <c r="I33" s="56"/>
-      <c r="J33" s="56"/>
+      <c r="D33" s="53"/>
+      <c r="E33" s="53"/>
+      <c r="F33" s="53"/>
+      <c r="G33" s="53"/>
+      <c r="H33" s="53"/>
+      <c r="I33" s="53"/>
+      <c r="J33" s="53"/>
     </row>
     <row r="34" s="7" customFormat="true" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="65" t="s">
-        <v>76</v>
-      </c>
+      <c r="A34" s="62"/>
       <c r="B34" s="16"/>
       <c r="C34" s="16"/>
-      <c r="D34" s="56"/>
-      <c r="E34" s="56"/>
-      <c r="F34" s="56"/>
-      <c r="G34" s="56"/>
-      <c r="H34" s="56"/>
-      <c r="I34" s="56"/>
-      <c r="J34" s="56"/>
+      <c r="D34" s="53"/>
+      <c r="E34" s="53"/>
+      <c r="F34" s="53"/>
+      <c r="G34" s="53"/>
+      <c r="H34" s="53"/>
+      <c r="I34" s="53"/>
+      <c r="J34" s="53"/>
       <c r="K34" s="1"/>
     </row>
     <row r="35" s="7" customFormat="true" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="65" t="s">
-        <v>77</v>
-      </c>
-      <c r="B35" s="56"/>
-      <c r="C35" s="56"/>
-      <c r="D35" s="56"/>
-      <c r="E35" s="56"/>
-      <c r="F35" s="56"/>
-      <c r="G35" s="56"/>
-      <c r="H35" s="56"/>
-      <c r="I35" s="56"/>
-      <c r="J35" s="56"/>
+      <c r="A35" s="62"/>
+      <c r="B35" s="53"/>
+      <c r="C35" s="53"/>
+      <c r="D35" s="53"/>
+      <c r="E35" s="53"/>
+      <c r="F35" s="53"/>
+      <c r="G35" s="53"/>
+      <c r="H35" s="53"/>
+      <c r="I35" s="53"/>
+      <c r="J35" s="53"/>
       <c r="K35" s="1"/>
     </row>
     <row r="36" s="7" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1857,7 +1455,7 @@
     </row>
     <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="12" t="s">
-        <v>78</v>
+        <v>56</v>
       </c>
       <c r="B37" s="12"/>
       <c r="C37" s="12"/>
@@ -1872,7 +1470,7 @@
     </row>
     <row r="38" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="7" t="s">
-        <v>79</v>
+        <v>57</v>
       </c>
       <c r="B38" s="7"/>
       <c r="C38" s="7"/>
@@ -1887,43 +1485,43 @@
     </row>
     <row r="39" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="7" t="s">
-        <v>80</v>
+        <v>58</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="41" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="27" t="s">
-        <v>81</v>
+        <v>59</v>
       </c>
       <c r="B41" s="27"/>
       <c r="C41" s="27"/>
       <c r="D41" s="27"/>
       <c r="E41" s="27"/>
       <c r="F41" s="27"/>
-      <c r="G41" s="66" t="s">
-        <v>82</v>
-      </c>
-      <c r="H41" s="66"/>
-      <c r="I41" s="66"/>
-      <c r="J41" s="66"/>
-      <c r="K41" s="66"/>
+      <c r="G41" s="63" t="s">
+        <v>60</v>
+      </c>
+      <c r="H41" s="63"/>
+      <c r="I41" s="63"/>
+      <c r="J41" s="63"/>
+      <c r="K41" s="63"/>
     </row>
     <row r="42" customFormat="false" ht="29.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="39" t="s">
-        <v>83</v>
-      </c>
-      <c r="B42" s="39"/>
-      <c r="C42" s="39"/>
-      <c r="D42" s="39"/>
-      <c r="E42" s="39"/>
-      <c r="F42" s="39"/>
-      <c r="G42" s="67" t="s">
-        <v>84</v>
-      </c>
-      <c r="H42" s="67"/>
-      <c r="I42" s="67"/>
-      <c r="J42" s="67"/>
-      <c r="K42" s="67"/>
+      <c r="A42" s="64" t="s">
+        <v>61</v>
+      </c>
+      <c r="B42" s="64"/>
+      <c r="C42" s="64"/>
+      <c r="D42" s="64"/>
+      <c r="E42" s="64"/>
+      <c r="F42" s="64"/>
+      <c r="G42" s="65" t="s">
+        <v>62</v>
+      </c>
+      <c r="H42" s="65"/>
+      <c r="I42" s="65"/>
+      <c r="J42" s="65"/>
+      <c r="K42" s="65"/>
     </row>
     <row r="43" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="7"/>

</xml_diff>

<commit_message>
Correçao nos subtitulos da planilha de demonstrativo financeiro.
</commit_message>
<xml_diff>
--- a/sme_ptrf_apps/static/cargas/modelo_demonstrativo_financeiro.xlsx
+++ b/sme_ptrf_apps/static/cargas/modelo_demonstrativo_financeiro.xlsx
@@ -71,7 +71,7 @@
     <t xml:space="preserve">09 - Repasse</t>
   </si>
   <si>
-    <t xml:space="preserve">10 - Rendimento</t>
+    <t xml:space="preserve">10 – Rendimento</t>
   </si>
   <si>
     <t xml:space="preserve">11 - Outras receitas</t>
@@ -92,7 +92,7 @@
     <t xml:space="preserve">BLOCO 3 - PAGAMENTOS EFETUADOS E DEMONSTRADOS</t>
   </si>
   <si>
-    <t xml:space="preserve">16 - Item</t>
+    <t xml:space="preserve">16 – Item</t>
   </si>
   <si>
     <t xml:space="preserve">Dados documento comprobatório da despesa</t>
@@ -104,7 +104,7 @@
     <t xml:space="preserve">Dados do pagamento</t>
   </si>
   <si>
-    <t xml:space="preserve">17 - Razão social</t>
+    <t xml:space="preserve">17 – Razão social</t>
   </si>
   <si>
     <t xml:space="preserve">18 - CNPJ ou CPF</t>
@@ -116,16 +116,16 @@
     <t xml:space="preserve">20 - Nº do documento</t>
   </si>
   <si>
-    <t xml:space="preserve">21 - Data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22 - Especificação do material ou serviço</t>
-  </si>
-  <si>
-    <t xml:space="preserve">23 - Tipo da despesa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">24 - Tipo de transação</t>
+    <t xml:space="preserve">21 – Data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22 – Especificação do material ou serviço</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23 - Tipo da despesa </t>
+  </si>
+  <si>
+    <t xml:space="preserve">24 -  Tipo de transação</t>
   </si>
   <si>
     <t xml:space="preserve">25 - Data</t>
@@ -137,13 +137,13 @@
     <t xml:space="preserve">BLOCO 4 - DÉBITOS NÃO DEMONSTRADOS NO EXTRATO DO PERÍODO</t>
   </si>
   <si>
-    <t xml:space="preserve">27 - Item</t>
+    <t xml:space="preserve">27 – Item</t>
   </si>
   <si>
     <t xml:space="preserve">Dados do pagamento (extrato bancário)</t>
   </si>
   <si>
-    <t xml:space="preserve">28 - Razão social</t>
+    <t xml:space="preserve">28 – Razão social</t>
   </si>
   <si>
     <t xml:space="preserve">29 - CNPJ ou CPF</t>
@@ -155,16 +155,16 @@
     <t xml:space="preserve">31 - Nº do documento</t>
   </si>
   <si>
-    <t xml:space="preserve">32 - Data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">33 - Especificação do material ou serviço</t>
-  </si>
-  <si>
-    <t xml:space="preserve">34 - Tipo da despesa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">35 - Tipo de transação</t>
+    <t xml:space="preserve">32 – Data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">33 – Especificação do material ou serviço</t>
+  </si>
+  <si>
+    <t xml:space="preserve">34 - Tipo da despesa </t>
+  </si>
+  <si>
+    <t xml:space="preserve">35 -  Tipo de transação</t>
   </si>
   <si>
     <t xml:space="preserve">36 - Data</t>
@@ -176,16 +176,16 @@
     <t xml:space="preserve">BLOCO 5 - CRÉDITOS NÃO DEMONSTRADOS NO EXTRATO DO PERÍODO</t>
   </si>
   <si>
-    <t xml:space="preserve">38 - Item</t>
+    <t xml:space="preserve">38 – Item</t>
   </si>
   <si>
     <t xml:space="preserve">39 - Tipo de receita</t>
   </si>
   <si>
-    <t xml:space="preserve">40 - Data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">41 - Valor </t>
+    <t xml:space="preserve">40 – Data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">41 - Valor</t>
   </si>
   <si>
     <t xml:space="preserve">BLOCO 6 - OBSERVAÇÃO</t>
@@ -392,7 +392,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="10">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -452,13 +452,6 @@
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right style="thin"/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right style="thin"/>
       <top style="thin"/>
       <bottom/>
       <diagonal/>
@@ -512,7 +505,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="57">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -672,55 +665,23 @@
     <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="true"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="4" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="true"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="true"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="true"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="true"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="true"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="8" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="true"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="true"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="8" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="true"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="true"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="true"/>
-    </xf>
     <xf numFmtId="168" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -741,13 +702,9 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="true"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="true"/>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
@@ -765,7 +722,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -773,7 +730,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -865,9 +822,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>59400</xdr:colOff>
+      <xdr:colOff>55800</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>129600</xdr:rowOff>
+      <xdr:rowOff>126000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -881,7 +838,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="66600" y="152280"/>
-          <a:ext cx="639720" cy="539280"/>
+          <a:ext cx="636120" cy="535680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -901,9 +858,9 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A2:Y1048576"/>
+  <dimension ref="A2:P1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
     </sheetView>
   </sheetViews>
@@ -1139,60 +1096,50 @@
       <c r="D19" s="41"/>
       <c r="E19" s="41"/>
       <c r="F19" s="41"/>
-      <c r="G19" s="42" t="s">
+      <c r="G19" s="41" t="s">
         <v>25</v>
       </c>
+      <c r="H19" s="41"/>
       <c r="I19" s="41" t="s">
         <v>26</v>
       </c>
       <c r="J19" s="41"/>
       <c r="K19" s="41"/>
     </row>
-    <row r="20" s="50" customFormat="true" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="40"/>
-      <c r="B20" s="43" t="s">
+    <row r="20" s="42" customFormat="true" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="43"/>
+      <c r="B20" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="C20" s="44" t="s">
+      <c r="C20" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="D20" s="44" t="s">
+      <c r="D20" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="E20" s="45" t="s">
+      <c r="E20" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="F20" s="46" t="s">
+      <c r="F20" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="G20" s="44" t="s">
+      <c r="G20" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="H20" s="44" t="s">
+      <c r="H20" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="I20" s="47" t="s">
+      <c r="I20" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="J20" s="45" t="s">
+      <c r="J20" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="K20" s="48" t="s">
+      <c r="K20" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="L20" s="49"/>
-      <c r="N20" s="51"/>
-      <c r="O20" s="51"/>
-      <c r="Q20" s="51"/>
-      <c r="R20" s="51"/>
-      <c r="S20" s="49"/>
-      <c r="U20" s="49"/>
-      <c r="V20" s="49"/>
-      <c r="W20" s="49"/>
-      <c r="X20" s="49"/>
-      <c r="Y20" s="49"/>
-    </row>
-    <row r="21" s="53" customFormat="true" ht="56.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="21" s="45" customFormat="true" ht="56.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="33" t="n">
         <v>1</v>
       </c>
@@ -1201,24 +1148,24 @@
       <c r="D21" s="38"/>
       <c r="E21" s="38"/>
       <c r="F21" s="38"/>
-      <c r="G21" s="52"/>
+      <c r="G21" s="44"/>
       <c r="H21" s="38"/>
       <c r="I21" s="18"/>
       <c r="J21" s="18"/>
       <c r="K21" s="18"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="54"/>
-      <c r="B22" s="53"/>
-      <c r="C22" s="53"/>
-      <c r="D22" s="53"/>
-      <c r="E22" s="53"/>
-      <c r="F22" s="53"/>
-      <c r="G22" s="53"/>
-      <c r="H22" s="53"/>
-      <c r="I22" s="53"/>
-      <c r="J22" s="53"/>
-      <c r="K22" s="53"/>
+      <c r="A22" s="46"/>
+      <c r="B22" s="45"/>
+      <c r="C22" s="45"/>
+      <c r="D22" s="45"/>
+      <c r="E22" s="45"/>
+      <c r="F22" s="45"/>
+      <c r="G22" s="45"/>
+      <c r="H22" s="45"/>
+      <c r="I22" s="45"/>
+      <c r="J22" s="45"/>
+      <c r="K22" s="45"/>
     </row>
     <row r="23" s="39" customFormat="true" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="12" t="s">
@@ -1246,61 +1193,51 @@
       <c r="D24" s="41"/>
       <c r="E24" s="41"/>
       <c r="F24" s="41"/>
-      <c r="G24" s="42" t="s">
+      <c r="G24" s="41" t="s">
         <v>25</v>
       </c>
+      <c r="H24" s="41"/>
       <c r="I24" s="41" t="s">
         <v>39</v>
       </c>
       <c r="J24" s="41"/>
       <c r="K24" s="41"/>
     </row>
-    <row r="25" s="50" customFormat="true" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="40"/>
-      <c r="B25" s="43" t="s">
+    <row r="25" s="42" customFormat="true" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="43"/>
+      <c r="B25" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="C25" s="44" t="s">
+      <c r="C25" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="D25" s="44" t="s">
+      <c r="D25" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="E25" s="45" t="s">
+      <c r="E25" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="F25" s="46" t="s">
+      <c r="F25" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="G25" s="44" t="s">
+      <c r="G25" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="H25" s="44" t="s">
+      <c r="H25" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="I25" s="47" t="s">
+      <c r="I25" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="J25" s="45" t="s">
+      <c r="J25" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="K25" s="48" t="s">
+      <c r="K25" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="L25" s="49"/>
-      <c r="N25" s="51"/>
-      <c r="O25" s="51"/>
-      <c r="Q25" s="51"/>
-      <c r="R25" s="51"/>
-      <c r="S25" s="49"/>
-      <c r="U25" s="49"/>
-      <c r="V25" s="49"/>
-      <c r="W25" s="49"/>
-      <c r="X25" s="49"/>
-      <c r="Y25" s="49"/>
-    </row>
-    <row r="26" s="56" customFormat="true" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="55"/>
+    </row>
+    <row r="26" s="48" customFormat="true" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="47"/>
       <c r="B26" s="18"/>
       <c r="C26" s="18"/>
       <c r="D26" s="18"/>
@@ -1313,17 +1250,17 @@
       <c r="K26" s="18"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="54"/>
-      <c r="B27" s="53"/>
-      <c r="C27" s="53"/>
-      <c r="D27" s="53"/>
-      <c r="E27" s="53"/>
-      <c r="F27" s="53"/>
-      <c r="G27" s="53"/>
-      <c r="H27" s="53"/>
-      <c r="I27" s="53"/>
-      <c r="J27" s="53"/>
-      <c r="K27" s="53"/>
+      <c r="A27" s="46"/>
+      <c r="B27" s="45"/>
+      <c r="C27" s="45"/>
+      <c r="D27" s="45"/>
+      <c r="E27" s="45"/>
+      <c r="F27" s="45"/>
+      <c r="G27" s="45"/>
+      <c r="H27" s="45"/>
+      <c r="I27" s="45"/>
+      <c r="J27" s="45"/>
+      <c r="K27" s="45"/>
     </row>
     <row r="28" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="12" t="s">
@@ -1340,52 +1277,52 @@
       <c r="J28" s="12"/>
       <c r="K28" s="12"/>
     </row>
-    <row r="29" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="57" t="s">
+    <row r="29" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A29" s="40" t="s">
         <v>51</v>
       </c>
-      <c r="B29" s="58" t="s">
+      <c r="B29" s="49" t="s">
         <v>52</v>
       </c>
-      <c r="C29" s="58"/>
-      <c r="D29" s="58"/>
-      <c r="E29" s="58"/>
-      <c r="F29" s="58" t="s">
+      <c r="C29" s="49"/>
+      <c r="D29" s="49"/>
+      <c r="E29" s="49"/>
+      <c r="F29" s="49" t="s">
         <v>53</v>
       </c>
-      <c r="G29" s="58"/>
-      <c r="H29" s="58" t="s">
+      <c r="G29" s="49"/>
+      <c r="H29" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="I29" s="58"/>
-      <c r="J29" s="58"/>
-      <c r="K29" s="58"/>
+      <c r="I29" s="26"/>
+      <c r="J29" s="26"/>
+      <c r="K29" s="26"/>
     </row>
     <row r="30" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="59"/>
-      <c r="B30" s="60"/>
-      <c r="C30" s="60"/>
-      <c r="D30" s="60"/>
-      <c r="E30" s="60"/>
-      <c r="F30" s="60"/>
-      <c r="G30" s="60"/>
-      <c r="H30" s="61"/>
-      <c r="I30" s="61"/>
-      <c r="J30" s="61"/>
-      <c r="K30" s="61"/>
+      <c r="A30" s="50"/>
+      <c r="B30" s="51"/>
+      <c r="C30" s="51"/>
+      <c r="D30" s="51"/>
+      <c r="E30" s="51"/>
+      <c r="F30" s="51"/>
+      <c r="G30" s="51"/>
+      <c r="H30" s="52"/>
+      <c r="I30" s="52"/>
+      <c r="J30" s="52"/>
+      <c r="K30" s="52"/>
     </row>
     <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="54"/>
-      <c r="B31" s="53"/>
-      <c r="C31" s="53"/>
-      <c r="D31" s="53"/>
-      <c r="E31" s="53"/>
-      <c r="F31" s="53"/>
-      <c r="G31" s="53"/>
-      <c r="H31" s="53"/>
-      <c r="I31" s="53"/>
-      <c r="J31" s="53"/>
-      <c r="K31" s="53"/>
+      <c r="A31" s="46"/>
+      <c r="B31" s="45"/>
+      <c r="C31" s="45"/>
+      <c r="D31" s="45"/>
+      <c r="E31" s="45"/>
+      <c r="F31" s="45"/>
+      <c r="G31" s="45"/>
+      <c r="H31" s="45"/>
+      <c r="I31" s="45"/>
+      <c r="J31" s="45"/>
+      <c r="K31" s="45"/>
     </row>
     <row r="32" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="12" t="s">
@@ -1403,41 +1340,41 @@
       <c r="K32" s="12"/>
     </row>
     <row r="33" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="62"/>
+      <c r="A33" s="53"/>
       <c r="B33" s="16"/>
       <c r="C33" s="16"/>
-      <c r="D33" s="53"/>
-      <c r="E33" s="53"/>
-      <c r="F33" s="53"/>
-      <c r="G33" s="53"/>
-      <c r="H33" s="53"/>
-      <c r="I33" s="53"/>
-      <c r="J33" s="53"/>
+      <c r="D33" s="45"/>
+      <c r="E33" s="45"/>
+      <c r="F33" s="45"/>
+      <c r="G33" s="45"/>
+      <c r="H33" s="45"/>
+      <c r="I33" s="45"/>
+      <c r="J33" s="45"/>
     </row>
     <row r="34" s="7" customFormat="true" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="62"/>
+      <c r="A34" s="53"/>
       <c r="B34" s="16"/>
       <c r="C34" s="16"/>
-      <c r="D34" s="53"/>
-      <c r="E34" s="53"/>
-      <c r="F34" s="53"/>
-      <c r="G34" s="53"/>
-      <c r="H34" s="53"/>
-      <c r="I34" s="53"/>
-      <c r="J34" s="53"/>
+      <c r="D34" s="45"/>
+      <c r="E34" s="45"/>
+      <c r="F34" s="45"/>
+      <c r="G34" s="45"/>
+      <c r="H34" s="45"/>
+      <c r="I34" s="45"/>
+      <c r="J34" s="45"/>
       <c r="K34" s="1"/>
     </row>
     <row r="35" s="7" customFormat="true" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="62"/>
-      <c r="B35" s="53"/>
-      <c r="C35" s="53"/>
-      <c r="D35" s="53"/>
-      <c r="E35" s="53"/>
-      <c r="F35" s="53"/>
-      <c r="G35" s="53"/>
-      <c r="H35" s="53"/>
-      <c r="I35" s="53"/>
-      <c r="J35" s="53"/>
+      <c r="A35" s="53"/>
+      <c r="B35" s="45"/>
+      <c r="C35" s="45"/>
+      <c r="D35" s="45"/>
+      <c r="E35" s="45"/>
+      <c r="F35" s="45"/>
+      <c r="G35" s="45"/>
+      <c r="H35" s="45"/>
+      <c r="I35" s="45"/>
+      <c r="J35" s="45"/>
       <c r="K35" s="1"/>
     </row>
     <row r="36" s="7" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1498,30 +1435,30 @@
       <c r="D41" s="27"/>
       <c r="E41" s="27"/>
       <c r="F41" s="27"/>
-      <c r="G41" s="63" t="s">
+      <c r="G41" s="54" t="s">
         <v>60</v>
       </c>
-      <c r="H41" s="63"/>
-      <c r="I41" s="63"/>
-      <c r="J41" s="63"/>
-      <c r="K41" s="63"/>
+      <c r="H41" s="54"/>
+      <c r="I41" s="54"/>
+      <c r="J41" s="54"/>
+      <c r="K41" s="54"/>
     </row>
     <row r="42" customFormat="false" ht="29.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="64" t="s">
+      <c r="A42" s="55" t="s">
         <v>61</v>
       </c>
-      <c r="B42" s="64"/>
-      <c r="C42" s="64"/>
-      <c r="D42" s="64"/>
-      <c r="E42" s="64"/>
-      <c r="F42" s="64"/>
-      <c r="G42" s="65" t="s">
+      <c r="B42" s="55"/>
+      <c r="C42" s="55"/>
+      <c r="D42" s="55"/>
+      <c r="E42" s="55"/>
+      <c r="F42" s="55"/>
+      <c r="G42" s="56" t="s">
         <v>62</v>
       </c>
-      <c r="H42" s="65"/>
-      <c r="I42" s="65"/>
-      <c r="J42" s="65"/>
-      <c r="K42" s="65"/>
+      <c r="H42" s="56"/>
+      <c r="I42" s="56"/>
+      <c r="J42" s="56"/>
+      <c r="K42" s="56"/>
     </row>
     <row r="43" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="7"/>

</xml_diff>

<commit_message>
Novas Correçoes no demonstrativo financeiro.
</commit_message>
<xml_diff>
--- a/sme_ptrf_apps/static/cargas/modelo_demonstrativo_financeiro.xlsx
+++ b/sme_ptrf_apps/static/cargas/modelo_demonstrativo_financeiro.xlsx
@@ -807,25 +807,127 @@
     <t xml:space="preserve">Valores do período</t>
   </si>
   <si>
-    <t xml:space="preserve">11 - Saldo reprogramado para o próximo período</t>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">11 - Saldo reprogramado para o próximo período
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">(08+09-10)</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Conciliação bancária</t>
   </si>
   <si>
-    <t xml:space="preserve">09 - Crédito no período</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10 - Despesa efetuada no período
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">09 - Crédito no período </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">(Campo 19 - Bloco 3)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">10 - Despesa efetuada no período
 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">12 - Despesa não demonstrada no extrato do período 
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">(Campo 31 - Bloco 4)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">12 - Despesa não demonstrada no extrato do período 
 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">13 - Saldo bancário ao final do período
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">(Campo 43 - Bloco 5)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">13 - Saldo bancário ao final do período
 </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">(11+12)</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Total </t>
@@ -849,7 +951,7 @@
     <t xml:space="preserve">18 – Valor</t>
   </si>
   <si>
-    <t xml:space="preserve">19 - TOTAL</t>
+    <t xml:space="preserve">19 – TOTAL</t>
   </si>
   <si>
     <t xml:space="preserve">BLOCO 4 - DESPESAS EFETUADAS NO PERÍODO </t>
@@ -894,7 +996,7 @@
     <t xml:space="preserve">BLOCO 5 - DESPESAS EFETUADAS E NÃO DEMONSTRADAS NO EXTRATO DO PERÍODO (ATUAL E ANTERIORES)</t>
   </si>
   <si>
-    <t xml:space="preserve">32 - Item</t>
+    <t xml:space="preserve">32 – Item</t>
   </si>
   <si>
     <t xml:space="preserve">33 – Razão social</t>
@@ -952,7 +1054,7 @@
     <numFmt numFmtId="170" formatCode="_-&quot;R$ &quot;* #,##0.00_-;&quot;-R$ &quot;* #,##0.00_-;_-&quot;R$ &quot;* \-??_-;_-@_-"/>
     <numFmt numFmtId="171" formatCode="#,##0.00"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1093,21 +1195,6 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <b val="true"/>
-      <sz val="8"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="8"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1265,7 +1352,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="123">
+  <cellXfs count="118">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1611,17 +1698,13 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1670,22 +1753,6 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1704,6 +1771,10 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1734,20 +1805,16 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="true"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1846,9 +1913,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>58320</xdr:colOff>
+      <xdr:colOff>54720</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>128520</xdr:rowOff>
+      <xdr:rowOff>124920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1862,7 +1929,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="66600" y="152280"/>
-          <a:ext cx="638640" cy="538200"/>
+          <a:ext cx="635040" cy="534600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1888,9 +1955,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>58320</xdr:colOff>
+      <xdr:colOff>54720</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>137880</xdr:rowOff>
+      <xdr:rowOff>134280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1904,7 +1971,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="66600" y="152280"/>
-          <a:ext cx="638640" cy="547560"/>
+          <a:ext cx="635040" cy="543960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3052,13 +3119,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:Y1048576"/>
+  <dimension ref="A1:Y1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G15" activeCellId="0" sqref="G15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A33" activeCellId="0" sqref="A33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="7.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.28"/>
@@ -3074,6 +3141,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="1" width="9.14"/>
   </cols>
   <sheetData>
+    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -3131,6 +3199,7 @@
       <c r="J7" s="85"/>
       <c r="K7" s="85"/>
     </row>
+    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="9" s="7" customFormat="true" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="12" t="s">
         <v>9</v>
@@ -3158,7 +3227,7 @@
       <c r="G10" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="H10" s="14" t="s">
+      <c r="H10" s="31" t="s">
         <v>89</v>
       </c>
       <c r="I10" s="15" t="s">
@@ -3176,10 +3245,11 @@
       <c r="F11" s="86"/>
       <c r="G11" s="87"/>
       <c r="H11" s="87"/>
-      <c r="I11" s="88"/>
-      <c r="J11" s="88"/>
-      <c r="K11" s="88"/>
-    </row>
+      <c r="I11" s="86"/>
+      <c r="J11" s="86"/>
+      <c r="K11" s="86"/>
+    </row>
+    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="13" s="40" customFormat="true" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="12" t="s">
         <v>15</v>
@@ -3196,80 +3266,81 @@
       <c r="K13" s="12"/>
     </row>
     <row r="14" s="7" customFormat="true" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="89" t="s">
+      <c r="A14" s="88" t="s">
         <v>90</v>
       </c>
-      <c r="B14" s="89"/>
-      <c r="C14" s="89" t="s">
+      <c r="B14" s="88"/>
+      <c r="C14" s="88" t="s">
         <v>91</v>
       </c>
-      <c r="D14" s="89"/>
-      <c r="E14" s="89" t="s">
+      <c r="D14" s="88"/>
+      <c r="E14" s="88" t="s">
         <v>92</v>
       </c>
-      <c r="F14" s="89"/>
-      <c r="G14" s="89" t="s">
+      <c r="F14" s="88"/>
+      <c r="G14" s="88" t="s">
         <v>93</v>
       </c>
-      <c r="H14" s="89"/>
-      <c r="I14" s="89"/>
-      <c r="J14" s="89"/>
-      <c r="K14" s="89"/>
+      <c r="H14" s="88"/>
+      <c r="I14" s="88"/>
+      <c r="J14" s="88"/>
+      <c r="K14" s="88"/>
     </row>
     <row r="15" s="7" customFormat="true" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="89"/>
-      <c r="B15" s="89"/>
-      <c r="C15" s="90" t="s">
+      <c r="A15" s="88"/>
+      <c r="B15" s="88"/>
+      <c r="C15" s="89" t="s">
         <v>94</v>
       </c>
-      <c r="D15" s="91" t="s">
+      <c r="D15" s="90" t="s">
         <v>95</v>
       </c>
-      <c r="E15" s="89"/>
-      <c r="F15" s="89"/>
-      <c r="G15" s="90" t="s">
+      <c r="E15" s="88"/>
+      <c r="F15" s="88"/>
+      <c r="G15" s="89" t="s">
         <v>96</v>
       </c>
-      <c r="H15" s="90"/>
-      <c r="I15" s="90" t="s">
+      <c r="H15" s="89"/>
+      <c r="I15" s="89" t="s">
         <v>97</v>
       </c>
-      <c r="J15" s="90"/>
-      <c r="K15" s="90"/>
-      <c r="L15" s="92"/>
+      <c r="J15" s="89"/>
+      <c r="K15" s="89"/>
+      <c r="L15" s="91"/>
     </row>
     <row r="16" s="7" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="93"/>
-      <c r="B16" s="93"/>
-      <c r="C16" s="94"/>
-      <c r="D16" s="94"/>
-      <c r="E16" s="94"/>
-      <c r="F16" s="95" t="s">
+      <c r="A16" s="92"/>
+      <c r="B16" s="92"/>
+      <c r="C16" s="93"/>
+      <c r="D16" s="93"/>
+      <c r="E16" s="93"/>
+      <c r="F16" s="94" t="s">
         <v>98</v>
       </c>
-      <c r="G16" s="93"/>
-      <c r="H16" s="93"/>
-      <c r="I16" s="93"/>
-      <c r="J16" s="93"/>
-      <c r="K16" s="96" t="s">
+      <c r="G16" s="92"/>
+      <c r="H16" s="92"/>
+      <c r="I16" s="92"/>
+      <c r="J16" s="92"/>
+      <c r="K16" s="95" t="s">
         <v>98</v>
       </c>
-      <c r="L16" s="92"/>
+      <c r="L16" s="91"/>
     </row>
     <row r="17" s="7" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="97"/>
-      <c r="B17" s="97"/>
-      <c r="C17" s="98"/>
-      <c r="D17" s="98"/>
-      <c r="E17" s="98"/>
-      <c r="F17" s="95"/>
-      <c r="G17" s="97"/>
-      <c r="H17" s="97"/>
-      <c r="I17" s="97"/>
-      <c r="J17" s="97"/>
-      <c r="K17" s="96"/>
-      <c r="L17" s="92"/>
-    </row>
+      <c r="A17" s="96"/>
+      <c r="B17" s="96"/>
+      <c r="C17" s="97"/>
+      <c r="D17" s="97"/>
+      <c r="E17" s="97"/>
+      <c r="F17" s="94"/>
+      <c r="G17" s="96"/>
+      <c r="H17" s="96"/>
+      <c r="I17" s="96"/>
+      <c r="J17" s="96"/>
+      <c r="K17" s="95"/>
+      <c r="L17" s="91"/>
+    </row>
+    <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="19" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="12" t="s">
         <v>99</v>
@@ -3286,451 +3357,409 @@
       <c r="K19" s="12"/>
     </row>
     <row r="20" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="99" t="s">
+      <c r="A20" s="98" t="s">
         <v>100</v>
       </c>
-      <c r="B20" s="99" t="s">
+      <c r="B20" s="98" t="s">
         <v>101</v>
       </c>
-      <c r="C20" s="99"/>
-      <c r="D20" s="99"/>
-      <c r="E20" s="99" t="s">
+      <c r="C20" s="98"/>
+      <c r="D20" s="98"/>
+      <c r="E20" s="98" t="s">
         <v>102</v>
       </c>
-      <c r="F20" s="99"/>
-      <c r="G20" s="99"/>
-      <c r="H20" s="99" t="s">
+      <c r="F20" s="98"/>
+      <c r="G20" s="98"/>
+      <c r="H20" s="98" t="s">
         <v>103</v>
       </c>
-      <c r="I20" s="99"/>
-      <c r="J20" s="99" t="s">
+      <c r="I20" s="98"/>
+      <c r="J20" s="98" t="s">
         <v>104</v>
       </c>
-      <c r="K20" s="99"/>
+      <c r="K20" s="98"/>
     </row>
     <row r="21" customFormat="false" ht="51.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="88"/>
-      <c r="B21" s="100"/>
-      <c r="C21" s="100"/>
-      <c r="D21" s="100"/>
-      <c r="E21" s="100"/>
-      <c r="F21" s="100"/>
-      <c r="G21" s="100"/>
-      <c r="H21" s="100"/>
-      <c r="I21" s="100"/>
-      <c r="J21" s="100"/>
-      <c r="K21" s="100"/>
-    </row>
-    <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="101"/>
-      <c r="B22" s="102"/>
-      <c r="C22" s="103"/>
-      <c r="D22" s="103"/>
-      <c r="E22" s="102"/>
-      <c r="F22" s="103"/>
-      <c r="G22" s="104"/>
-      <c r="H22" s="102"/>
-      <c r="I22" s="104"/>
-      <c r="J22" s="102"/>
-      <c r="K22" s="104"/>
-    </row>
-    <row r="23" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="105" t="s">
+      <c r="A21" s="86"/>
+      <c r="B21" s="99"/>
+      <c r="C21" s="99"/>
+      <c r="D21" s="99"/>
+      <c r="E21" s="99"/>
+      <c r="F21" s="99"/>
+      <c r="G21" s="99"/>
+      <c r="H21" s="99"/>
+      <c r="I21" s="99"/>
+      <c r="J21" s="99"/>
+      <c r="K21" s="99"/>
+    </row>
+    <row r="22" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="100" t="s">
         <v>105</v>
       </c>
-      <c r="B23" s="105"/>
-      <c r="C23" s="105"/>
-      <c r="D23" s="105"/>
-      <c r="E23" s="105"/>
-      <c r="F23" s="105"/>
-      <c r="G23" s="105"/>
-      <c r="H23" s="105"/>
-      <c r="I23" s="105"/>
-      <c r="J23" s="106"/>
-      <c r="K23" s="106"/>
-    </row>
-    <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="107"/>
-      <c r="B24" s="108"/>
-      <c r="C24" s="108"/>
-      <c r="D24" s="108"/>
-      <c r="E24" s="108"/>
-      <c r="F24" s="108"/>
-      <c r="G24" s="108"/>
-      <c r="H24" s="109"/>
-      <c r="I24" s="109"/>
-      <c r="J24" s="109"/>
-      <c r="K24" s="109"/>
-    </row>
-    <row r="25" s="40" customFormat="true" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="12" t="s">
+      <c r="B22" s="100"/>
+      <c r="C22" s="100"/>
+      <c r="D22" s="100"/>
+      <c r="E22" s="100"/>
+      <c r="F22" s="100"/>
+      <c r="G22" s="100"/>
+      <c r="H22" s="100"/>
+      <c r="I22" s="100"/>
+      <c r="J22" s="101"/>
+      <c r="K22" s="101"/>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="102"/>
+      <c r="B23" s="103"/>
+      <c r="C23" s="103"/>
+      <c r="D23" s="103"/>
+      <c r="E23" s="103"/>
+      <c r="F23" s="103"/>
+      <c r="G23" s="103"/>
+      <c r="H23" s="104"/>
+      <c r="I23" s="104"/>
+      <c r="J23" s="104"/>
+      <c r="K23" s="104"/>
+    </row>
+    <row r="24" s="40" customFormat="true" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="B25" s="12"/>
-      <c r="C25" s="12"/>
-      <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
-      <c r="G25" s="12"/>
-      <c r="H25" s="12"/>
-      <c r="I25" s="12"/>
-      <c r="J25" s="12"/>
-      <c r="K25" s="12"/>
-    </row>
-    <row r="26" s="111" customFormat="true" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="99" t="s">
+      <c r="B24" s="12"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="12"/>
+      <c r="J24" s="12"/>
+      <c r="K24" s="12"/>
+    </row>
+    <row r="25" s="107" customFormat="true" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="105" t="s">
         <v>107</v>
       </c>
-      <c r="B26" s="110" t="s">
+      <c r="B25" s="106" t="s">
         <v>40</v>
       </c>
-      <c r="C26" s="110"/>
-      <c r="D26" s="110"/>
-      <c r="E26" s="110"/>
-      <c r="F26" s="110"/>
-      <c r="G26" s="110" t="s">
+      <c r="C25" s="106"/>
+      <c r="D25" s="106"/>
+      <c r="E25" s="106"/>
+      <c r="F25" s="106"/>
+      <c r="G25" s="106" t="s">
         <v>41</v>
       </c>
-      <c r="H26" s="110"/>
-      <c r="I26" s="110" t="s">
+      <c r="H25" s="106"/>
+      <c r="I25" s="106" t="s">
         <v>42</v>
       </c>
-      <c r="J26" s="110"/>
-      <c r="K26" s="110"/>
-    </row>
-    <row r="27" s="114" customFormat="true" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="41"/>
-      <c r="B27" s="99" t="s">
+      <c r="J25" s="106"/>
+      <c r="K25" s="106"/>
+    </row>
+    <row r="26" s="110" customFormat="true" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="38"/>
+      <c r="B26" s="98" t="s">
         <v>108</v>
       </c>
-      <c r="C27" s="112" t="s">
+      <c r="C26" s="108" t="s">
         <v>109</v>
       </c>
-      <c r="D27" s="99" t="s">
+      <c r="D26" s="98" t="s">
         <v>110</v>
       </c>
-      <c r="E27" s="99" t="s">
+      <c r="E26" s="98" t="s">
         <v>111</v>
       </c>
-      <c r="F27" s="99" t="s">
+      <c r="F26" s="98" t="s">
         <v>112</v>
       </c>
-      <c r="G27" s="99" t="s">
+      <c r="G26" s="98" t="s">
         <v>113</v>
       </c>
-      <c r="H27" s="99" t="s">
+      <c r="H26" s="98" t="s">
         <v>114</v>
       </c>
-      <c r="I27" s="99" t="s">
+      <c r="I26" s="98" t="s">
         <v>115</v>
       </c>
-      <c r="J27" s="99" t="s">
+      <c r="J26" s="98" t="s">
         <v>116</v>
       </c>
-      <c r="K27" s="99" t="s">
+      <c r="K26" s="98" t="s">
         <v>117</v>
       </c>
-      <c r="L27" s="113"/>
-      <c r="N27" s="115"/>
-      <c r="O27" s="115"/>
-      <c r="Q27" s="115"/>
-      <c r="R27" s="115"/>
-      <c r="S27" s="113"/>
-      <c r="U27" s="113"/>
-      <c r="V27" s="113"/>
-      <c r="W27" s="113"/>
-      <c r="X27" s="113"/>
-      <c r="Y27" s="113"/>
-    </row>
-    <row r="28" s="20" customFormat="true" ht="51.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="116"/>
-      <c r="B28" s="87"/>
-      <c r="C28" s="87"/>
-      <c r="D28" s="87"/>
-      <c r="E28" s="87"/>
-      <c r="F28" s="87"/>
-      <c r="G28" s="87"/>
-      <c r="H28" s="87"/>
-      <c r="I28" s="87"/>
-      <c r="J28" s="87"/>
-      <c r="K28" s="87"/>
-    </row>
-    <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="101"/>
-      <c r="B29" s="117"/>
-      <c r="C29" s="117"/>
-      <c r="D29" s="117"/>
-      <c r="E29" s="117"/>
-      <c r="F29" s="117"/>
-      <c r="G29" s="117"/>
-      <c r="H29" s="117"/>
-      <c r="I29" s="117"/>
-      <c r="J29" s="117"/>
-      <c r="K29" s="117"/>
-    </row>
-    <row r="30" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="105" t="s">
+      <c r="L26" s="109"/>
+      <c r="N26" s="111"/>
+      <c r="O26" s="111"/>
+      <c r="Q26" s="111"/>
+      <c r="R26" s="111"/>
+      <c r="S26" s="109"/>
+      <c r="U26" s="109"/>
+      <c r="V26" s="109"/>
+      <c r="W26" s="109"/>
+      <c r="X26" s="109"/>
+      <c r="Y26" s="109"/>
+    </row>
+    <row r="27" s="20" customFormat="true" ht="51.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="112"/>
+      <c r="B27" s="87"/>
+      <c r="C27" s="87"/>
+      <c r="D27" s="87"/>
+      <c r="E27" s="87"/>
+      <c r="F27" s="87"/>
+      <c r="G27" s="87"/>
+      <c r="H27" s="87"/>
+      <c r="I27" s="87"/>
+      <c r="J27" s="87"/>
+      <c r="K27" s="87"/>
+    </row>
+    <row r="28" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A28" s="100" t="s">
         <v>118</v>
       </c>
-      <c r="B30" s="105"/>
-      <c r="C30" s="105"/>
-      <c r="D30" s="105"/>
-      <c r="E30" s="105"/>
-      <c r="F30" s="105"/>
-      <c r="G30" s="105"/>
-      <c r="H30" s="105"/>
-      <c r="I30" s="105"/>
-      <c r="J30" s="106"/>
-      <c r="K30" s="106"/>
-      <c r="M30" s="118"/>
-    </row>
-    <row r="32" s="40" customFormat="true" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="12" t="s">
+      <c r="B28" s="100"/>
+      <c r="C28" s="100"/>
+      <c r="D28" s="100"/>
+      <c r="E28" s="100"/>
+      <c r="F28" s="100"/>
+      <c r="G28" s="100"/>
+      <c r="H28" s="100"/>
+      <c r="I28" s="100"/>
+      <c r="J28" s="101"/>
+      <c r="K28" s="101"/>
+      <c r="M28" s="113"/>
+    </row>
+    <row r="30" s="40" customFormat="true" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A30" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="B32" s="12"/>
-      <c r="C32" s="12"/>
-      <c r="D32" s="12"/>
-      <c r="E32" s="12"/>
-      <c r="F32" s="12"/>
-      <c r="G32" s="12"/>
-      <c r="H32" s="12"/>
-      <c r="I32" s="12"/>
-      <c r="J32" s="12"/>
-      <c r="K32" s="12"/>
-    </row>
-    <row r="33" s="111" customFormat="true" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="41" t="s">
+      <c r="B30" s="12"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="12"/>
+      <c r="H30" s="12"/>
+      <c r="I30" s="12"/>
+      <c r="J30" s="12"/>
+      <c r="K30" s="12"/>
+    </row>
+    <row r="31" s="107" customFormat="true" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A31" s="105" t="s">
         <v>120</v>
       </c>
-      <c r="B33" s="42" t="s">
+      <c r="B31" s="106" t="s">
         <v>40</v>
       </c>
-      <c r="C33" s="42"/>
-      <c r="D33" s="42"/>
-      <c r="E33" s="42"/>
-      <c r="F33" s="42"/>
-      <c r="G33" s="43" t="s">
+      <c r="C31" s="106"/>
+      <c r="D31" s="106"/>
+      <c r="E31" s="106"/>
+      <c r="F31" s="106"/>
+      <c r="G31" s="106" t="s">
         <v>41</v>
       </c>
-      <c r="H33" s="43"/>
-      <c r="I33" s="42" t="s">
+      <c r="H31" s="106"/>
+      <c r="I31" s="106" t="s">
         <v>42</v>
       </c>
-      <c r="J33" s="42"/>
-      <c r="K33" s="42"/>
-    </row>
-    <row r="34" s="114" customFormat="true" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="41"/>
-      <c r="B34" s="99" t="s">
+      <c r="J31" s="106"/>
+      <c r="K31" s="106"/>
+    </row>
+    <row r="32" s="110" customFormat="true" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A32" s="114"/>
+      <c r="B32" s="98" t="s">
         <v>121</v>
       </c>
-      <c r="C34" s="112" t="s">
+      <c r="C32" s="108" t="s">
         <v>122</v>
       </c>
-      <c r="D34" s="99" t="s">
+      <c r="D32" s="98" t="s">
         <v>123</v>
       </c>
-      <c r="E34" s="99" t="s">
+      <c r="E32" s="98" t="s">
         <v>124</v>
       </c>
-      <c r="F34" s="99" t="s">
+      <c r="F32" s="98" t="s">
         <v>125</v>
       </c>
-      <c r="G34" s="99" t="s">
+      <c r="G32" s="98" t="s">
         <v>126</v>
       </c>
-      <c r="H34" s="99" t="s">
+      <c r="H32" s="98" t="s">
         <v>127</v>
       </c>
-      <c r="I34" s="99" t="s">
+      <c r="I32" s="98" t="s">
         <v>128</v>
       </c>
-      <c r="J34" s="99" t="s">
+      <c r="J32" s="98" t="s">
         <v>129</v>
       </c>
-      <c r="K34" s="99" t="s">
+      <c r="K32" s="98" t="s">
         <v>130</v>
       </c>
-      <c r="L34" s="113"/>
-      <c r="N34" s="115"/>
-      <c r="O34" s="115"/>
-      <c r="Q34" s="115"/>
-      <c r="R34" s="115"/>
-      <c r="S34" s="113"/>
-      <c r="U34" s="113"/>
-      <c r="V34" s="113"/>
-      <c r="W34" s="113"/>
-      <c r="X34" s="113"/>
-      <c r="Y34" s="113"/>
-    </row>
-    <row r="35" s="20" customFormat="true" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="116"/>
-      <c r="B35" s="87"/>
-      <c r="C35" s="87"/>
-      <c r="D35" s="87"/>
-      <c r="E35" s="87"/>
-      <c r="F35" s="87"/>
-      <c r="G35" s="87"/>
-      <c r="H35" s="87"/>
-      <c r="I35" s="87"/>
-      <c r="J35" s="87"/>
-      <c r="K35" s="87"/>
-    </row>
-    <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="119"/>
-      <c r="B36" s="120"/>
-      <c r="C36" s="117"/>
-      <c r="D36" s="117"/>
-      <c r="E36" s="117"/>
-      <c r="F36" s="117"/>
-      <c r="G36" s="117"/>
-      <c r="H36" s="117"/>
-      <c r="I36" s="117"/>
-      <c r="J36" s="117"/>
-      <c r="K36" s="117"/>
-    </row>
-    <row r="37" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="105" t="s">
+      <c r="L32" s="109"/>
+      <c r="N32" s="111"/>
+      <c r="O32" s="111"/>
+      <c r="Q32" s="111"/>
+      <c r="R32" s="111"/>
+      <c r="S32" s="109"/>
+      <c r="U32" s="109"/>
+      <c r="V32" s="109"/>
+      <c r="W32" s="109"/>
+      <c r="X32" s="109"/>
+      <c r="Y32" s="109"/>
+    </row>
+    <row r="33" s="20" customFormat="true" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A33" s="115"/>
+      <c r="B33" s="87"/>
+      <c r="C33" s="87"/>
+      <c r="D33" s="87"/>
+      <c r="E33" s="87"/>
+      <c r="F33" s="87"/>
+      <c r="G33" s="87"/>
+      <c r="H33" s="87"/>
+      <c r="I33" s="87"/>
+      <c r="J33" s="87"/>
+      <c r="K33" s="87"/>
+    </row>
+    <row r="34" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A34" s="100" t="s">
         <v>131</v>
       </c>
-      <c r="B37" s="105"/>
-      <c r="C37" s="105"/>
-      <c r="D37" s="105"/>
-      <c r="E37" s="105"/>
-      <c r="F37" s="105"/>
-      <c r="G37" s="105"/>
-      <c r="H37" s="105"/>
-      <c r="I37" s="105"/>
-      <c r="J37" s="106"/>
-      <c r="K37" s="106"/>
-      <c r="M37" s="118"/>
-    </row>
-    <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="65"/>
-      <c r="B38" s="109"/>
-      <c r="C38" s="109"/>
-      <c r="D38" s="109"/>
-      <c r="E38" s="109"/>
-      <c r="F38" s="109"/>
-      <c r="G38" s="109"/>
-      <c r="H38" s="109"/>
-      <c r="I38" s="109"/>
-      <c r="J38" s="109"/>
-      <c r="K38" s="121"/>
-    </row>
-    <row r="39" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="12" t="s">
+      <c r="B34" s="100"/>
+      <c r="C34" s="100"/>
+      <c r="D34" s="100"/>
+      <c r="E34" s="100"/>
+      <c r="F34" s="100"/>
+      <c r="G34" s="100"/>
+      <c r="H34" s="100"/>
+      <c r="I34" s="100"/>
+      <c r="J34" s="101"/>
+      <c r="K34" s="101"/>
+      <c r="M34" s="113"/>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="65"/>
+      <c r="B35" s="104"/>
+      <c r="C35" s="104"/>
+      <c r="D35" s="104"/>
+      <c r="E35" s="104"/>
+      <c r="F35" s="104"/>
+      <c r="G35" s="104"/>
+      <c r="H35" s="104"/>
+      <c r="I35" s="104"/>
+      <c r="J35" s="104"/>
+      <c r="K35" s="116"/>
+    </row>
+    <row r="36" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A36" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="B39" s="12"/>
-      <c r="C39" s="12"/>
-      <c r="D39" s="12"/>
-      <c r="E39" s="12"/>
-      <c r="F39" s="12"/>
-      <c r="G39" s="12"/>
-      <c r="H39" s="12"/>
-      <c r="I39" s="12"/>
-      <c r="J39" s="12"/>
-      <c r="K39" s="12"/>
-    </row>
-    <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="118"/>
-      <c r="B40" s="7"/>
-      <c r="C40" s="7"/>
-    </row>
-    <row r="41" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="118"/>
-      <c r="B41" s="7"/>
-      <c r="C41" s="7"/>
-    </row>
-    <row r="42" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="118"/>
-    </row>
-    <row r="44" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="12" t="s">
+      <c r="B36" s="12"/>
+      <c r="C36" s="12"/>
+      <c r="D36" s="12"/>
+      <c r="E36" s="12"/>
+      <c r="F36" s="12"/>
+      <c r="G36" s="12"/>
+      <c r="H36" s="12"/>
+      <c r="I36" s="12"/>
+      <c r="J36" s="12"/>
+      <c r="K36" s="12"/>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="113"/>
+      <c r="B37" s="7"/>
+      <c r="C37" s="7"/>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="113"/>
+      <c r="B38" s="7"/>
+      <c r="C38" s="7"/>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="113"/>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="B44" s="12"/>
-      <c r="C44" s="12"/>
-      <c r="D44" s="12"/>
-      <c r="E44" s="12"/>
-      <c r="F44" s="12"/>
-      <c r="G44" s="12"/>
-      <c r="H44" s="12"/>
-      <c r="I44" s="12"/>
-      <c r="J44" s="12"/>
-      <c r="K44" s="12"/>
-    </row>
-    <row r="45" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="7" t="s">
+      <c r="B41" s="12"/>
+      <c r="C41" s="12"/>
+      <c r="D41" s="12"/>
+      <c r="E41" s="12"/>
+      <c r="F41" s="12"/>
+      <c r="G41" s="12"/>
+      <c r="H41" s="12"/>
+      <c r="I41" s="12"/>
+      <c r="J41" s="12"/>
+      <c r="K41" s="12"/>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="B45" s="7"/>
-      <c r="C45" s="7"/>
-      <c r="D45" s="7"/>
-      <c r="E45" s="7"/>
-      <c r="F45" s="7"/>
-      <c r="G45" s="7"/>
-      <c r="H45" s="7"/>
-      <c r="I45" s="7"/>
-      <c r="J45" s="7"/>
-      <c r="K45" s="7"/>
-    </row>
-    <row r="46" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="7" t="s">
+      <c r="B42" s="7"/>
+      <c r="C42" s="7"/>
+      <c r="D42" s="7"/>
+      <c r="E42" s="7"/>
+      <c r="F42" s="7"/>
+      <c r="G42" s="7"/>
+      <c r="H42" s="7"/>
+      <c r="I42" s="7"/>
+      <c r="J42" s="7"/>
+      <c r="K42" s="7"/>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="7" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A48" s="27" t="s">
+    <row r="45" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A45" s="27" t="s">
         <v>132</v>
       </c>
-      <c r="B48" s="27"/>
-      <c r="C48" s="27"/>
-      <c r="D48" s="27"/>
-      <c r="E48" s="27"/>
-      <c r="F48" s="27"/>
-      <c r="G48" s="79" t="s">
+      <c r="B45" s="27"/>
+      <c r="C45" s="27"/>
+      <c r="D45" s="27"/>
+      <c r="E45" s="27"/>
+      <c r="F45" s="27"/>
+      <c r="G45" s="79" t="s">
         <v>133</v>
       </c>
-      <c r="H48" s="79"/>
-      <c r="I48" s="79"/>
-      <c r="J48" s="79"/>
-      <c r="K48" s="79"/>
-    </row>
-    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="39"/>
-      <c r="B49" s="39"/>
-      <c r="C49" s="39"/>
-      <c r="D49" s="39"/>
-      <c r="E49" s="39"/>
-      <c r="F49" s="39"/>
-      <c r="G49" s="80"/>
-      <c r="H49" s="80"/>
-      <c r="I49" s="80"/>
-      <c r="J49" s="80"/>
-      <c r="K49" s="80"/>
-    </row>
-    <row r="50" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="7"/>
-      <c r="B50" s="7"/>
-      <c r="C50" s="7"/>
-      <c r="D50" s="7"/>
-      <c r="E50" s="7"/>
-      <c r="F50" s="7"/>
-      <c r="G50" s="7"/>
-      <c r="H50" s="7"/>
-      <c r="I50" s="7"/>
-      <c r="J50" s="7"/>
-      <c r="K50" s="7"/>
-    </row>
-    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="122"/>
-    </row>
-    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="H45" s="79"/>
+      <c r="I45" s="79"/>
+      <c r="J45" s="79"/>
+      <c r="K45" s="79"/>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="39"/>
+      <c r="B46" s="39"/>
+      <c r="C46" s="39"/>
+      <c r="D46" s="39"/>
+      <c r="E46" s="39"/>
+      <c r="F46" s="39"/>
+      <c r="G46" s="80"/>
+      <c r="H46" s="80"/>
+      <c r="I46" s="80"/>
+      <c r="J46" s="80"/>
+      <c r="K46" s="80"/>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="7"/>
+      <c r="B47" s="7"/>
+      <c r="C47" s="7"/>
+      <c r="D47" s="7"/>
+      <c r="E47" s="7"/>
+      <c r="F47" s="7"/>
+      <c r="G47" s="7"/>
+      <c r="H47" s="7"/>
+      <c r="I47" s="7"/>
+      <c r="J47" s="7"/>
+      <c r="K47" s="7"/>
+    </row>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="117"/>
+    </row>
     <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -3773,26 +3802,26 @@
     <mergeCell ref="E21:G21"/>
     <mergeCell ref="H21:I21"/>
     <mergeCell ref="J21:K21"/>
-    <mergeCell ref="A23:I23"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="A25:K25"/>
-    <mergeCell ref="B26:F26"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="I26:K26"/>
-    <mergeCell ref="A30:I30"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="A32:K32"/>
-    <mergeCell ref="B33:F33"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="I33:K33"/>
-    <mergeCell ref="A37:I37"/>
-    <mergeCell ref="J37:K37"/>
-    <mergeCell ref="A39:K39"/>
-    <mergeCell ref="A44:K44"/>
-    <mergeCell ref="A48:F48"/>
-    <mergeCell ref="G48:K48"/>
-    <mergeCell ref="A49:F49"/>
-    <mergeCell ref="G49:K49"/>
+    <mergeCell ref="A22:I22"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="A24:K24"/>
+    <mergeCell ref="B25:F25"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="I25:K25"/>
+    <mergeCell ref="A28:I28"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="A30:K30"/>
+    <mergeCell ref="B31:F31"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="I31:K31"/>
+    <mergeCell ref="A34:I34"/>
+    <mergeCell ref="J34:K34"/>
+    <mergeCell ref="A36:K36"/>
+    <mergeCell ref="A41:K41"/>
+    <mergeCell ref="A45:F45"/>
+    <mergeCell ref="G45:K45"/>
+    <mergeCell ref="A46:F46"/>
+    <mergeCell ref="G46:K46"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Correção nome sheet planilha do demonstrativo financeiro.
</commit_message>
<xml_diff>
--- a/sme_ptrf_apps/static/cargas/modelo_demonstrativo_financeiro.xlsx
+++ b/sme_ptrf_apps/static/cargas/modelo_demonstrativo_financeiro.xlsx
@@ -9,7 +9,7 @@
   </bookViews>
   <sheets>
     <sheet name="Atual" sheetId="1" state="hidden" r:id="rId2"/>
-    <sheet name="MELHORIA" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Demonstrativo" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -1913,9 +1913,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>54720</xdr:colOff>
+      <xdr:colOff>54360</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>124920</xdr:rowOff>
+      <xdr:rowOff>124560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1929,7 +1929,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="66600" y="152280"/>
-          <a:ext cx="635040" cy="534600"/>
+          <a:ext cx="634680" cy="534240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1955,9 +1955,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>54720</xdr:colOff>
+      <xdr:colOff>54360</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>134280</xdr:rowOff>
+      <xdr:rowOff>133920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1971,7 +1971,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="66600" y="152280"/>
-          <a:ext cx="635040" cy="543960"/>
+          <a:ext cx="634680" cy="543600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3121,7 +3121,7 @@
   </sheetPr>
   <dimension ref="A1:Y1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A33" activeCellId="0" sqref="A33"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Atualizaçao do modelo demonstrativo financeiro.
</commit_message>
<xml_diff>
--- a/sme_ptrf_apps/static/cargas/modelo_demonstrativo_financeiro.xlsx
+++ b/sme_ptrf_apps/static/cargas/modelo_demonstrativo_financeiro.xlsx
@@ -1913,9 +1913,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>54360</xdr:colOff>
+      <xdr:colOff>54000</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>124560</xdr:rowOff>
+      <xdr:rowOff>124200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1929,7 +1929,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="66600" y="152280"/>
-          <a:ext cx="634680" cy="534240"/>
+          <a:ext cx="634320" cy="533880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1955,9 +1955,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>54360</xdr:colOff>
+      <xdr:colOff>54000</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>133920</xdr:rowOff>
+      <xdr:rowOff>133560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1971,7 +1971,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="66600" y="152280"/>
-          <a:ext cx="634680" cy="543600"/>
+          <a:ext cx="634320" cy="543240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3121,8 +3121,8 @@
   </sheetPr>
   <dimension ref="A1:Y1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A33" activeCellId="0" sqref="A33"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A27" activeCellId="0" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3327,349 +3327,358 @@
       <c r="L16" s="91"/>
     </row>
     <row r="17" s="7" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="96"/>
-      <c r="B17" s="96"/>
-      <c r="C17" s="97"/>
-      <c r="D17" s="97"/>
-      <c r="E17" s="97"/>
+      <c r="A17" s="92"/>
+      <c r="B17" s="92"/>
+      <c r="C17" s="93"/>
+      <c r="D17" s="93"/>
+      <c r="E17" s="93"/>
       <c r="F17" s="94"/>
-      <c r="G17" s="96"/>
-      <c r="H17" s="96"/>
-      <c r="I17" s="96"/>
-      <c r="J17" s="96"/>
+      <c r="G17" s="92"/>
+      <c r="H17" s="92"/>
+      <c r="I17" s="92"/>
+      <c r="J17" s="92"/>
       <c r="K17" s="95"/>
       <c r="L17" s="91"/>
     </row>
-    <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="19" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="12" t="s">
+    <row r="18" s="7" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="96"/>
+      <c r="B18" s="96"/>
+      <c r="C18" s="97"/>
+      <c r="D18" s="97"/>
+      <c r="E18" s="97"/>
+      <c r="F18" s="94"/>
+      <c r="G18" s="96"/>
+      <c r="H18" s="96"/>
+      <c r="I18" s="96"/>
+      <c r="J18" s="96"/>
+      <c r="K18" s="95"/>
+      <c r="L18" s="91"/>
+    </row>
+    <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="20" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="B19" s="12"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="12"/>
-      <c r="J19" s="12"/>
-      <c r="K19" s="12"/>
-    </row>
-    <row r="20" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="98" t="s">
+      <c r="B20" s="12"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="12"/>
+      <c r="K20" s="12"/>
+    </row>
+    <row r="21" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="98" t="s">
         <v>100</v>
       </c>
-      <c r="B20" s="98" t="s">
+      <c r="B21" s="98" t="s">
         <v>101</v>
       </c>
-      <c r="C20" s="98"/>
-      <c r="D20" s="98"/>
-      <c r="E20" s="98" t="s">
+      <c r="C21" s="98"/>
+      <c r="D21" s="98"/>
+      <c r="E21" s="98" t="s">
         <v>102</v>
       </c>
-      <c r="F20" s="98"/>
-      <c r="G20" s="98"/>
-      <c r="H20" s="98" t="s">
+      <c r="F21" s="98"/>
+      <c r="G21" s="98"/>
+      <c r="H21" s="98" t="s">
         <v>103</v>
       </c>
-      <c r="I20" s="98"/>
-      <c r="J20" s="98" t="s">
+      <c r="I21" s="98"/>
+      <c r="J21" s="98" t="s">
         <v>104</v>
       </c>
-      <c r="K20" s="98"/>
-    </row>
-    <row r="21" customFormat="false" ht="51.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="86"/>
-      <c r="B21" s="99"/>
-      <c r="C21" s="99"/>
-      <c r="D21" s="99"/>
-      <c r="E21" s="99"/>
-      <c r="F21" s="99"/>
-      <c r="G21" s="99"/>
-      <c r="H21" s="99"/>
-      <c r="I21" s="99"/>
-      <c r="J21" s="99"/>
-      <c r="K21" s="99"/>
-    </row>
-    <row r="22" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="100" t="s">
+      <c r="K21" s="98"/>
+    </row>
+    <row r="22" customFormat="false" ht="51.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="86"/>
+      <c r="B22" s="99"/>
+      <c r="C22" s="99"/>
+      <c r="D22" s="99"/>
+      <c r="E22" s="99"/>
+      <c r="F22" s="99"/>
+      <c r="G22" s="99"/>
+      <c r="H22" s="99"/>
+      <c r="I22" s="99"/>
+      <c r="J22" s="99"/>
+      <c r="K22" s="99"/>
+    </row>
+    <row r="23" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="100" t="s">
         <v>105</v>
       </c>
-      <c r="B22" s="100"/>
-      <c r="C22" s="100"/>
-      <c r="D22" s="100"/>
-      <c r="E22" s="100"/>
-      <c r="F22" s="100"/>
-      <c r="G22" s="100"/>
-      <c r="H22" s="100"/>
-      <c r="I22" s="100"/>
-      <c r="J22" s="101"/>
-      <c r="K22" s="101"/>
-    </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="102"/>
-      <c r="B23" s="103"/>
-      <c r="C23" s="103"/>
-      <c r="D23" s="103"/>
-      <c r="E23" s="103"/>
-      <c r="F23" s="103"/>
-      <c r="G23" s="103"/>
-      <c r="H23" s="104"/>
-      <c r="I23" s="104"/>
-      <c r="J23" s="104"/>
-      <c r="K23" s="104"/>
-    </row>
-    <row r="24" s="40" customFormat="true" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="12" t="s">
+      <c r="B23" s="100"/>
+      <c r="C23" s="100"/>
+      <c r="D23" s="100"/>
+      <c r="E23" s="100"/>
+      <c r="F23" s="100"/>
+      <c r="G23" s="100"/>
+      <c r="H23" s="100"/>
+      <c r="I23" s="100"/>
+      <c r="J23" s="101"/>
+      <c r="K23" s="101"/>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="102"/>
+      <c r="B24" s="103"/>
+      <c r="C24" s="103"/>
+      <c r="D24" s="103"/>
+      <c r="E24" s="103"/>
+      <c r="F24" s="103"/>
+      <c r="G24" s="103"/>
+      <c r="H24" s="104"/>
+      <c r="I24" s="104"/>
+      <c r="J24" s="104"/>
+      <c r="K24" s="104"/>
+    </row>
+    <row r="25" s="40" customFormat="true" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="B24" s="12"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="12"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
-      <c r="G24" s="12"/>
-      <c r="H24" s="12"/>
-      <c r="I24" s="12"/>
-      <c r="J24" s="12"/>
-      <c r="K24" s="12"/>
-    </row>
-    <row r="25" s="107" customFormat="true" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="105" t="s">
+      <c r="B25" s="12"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="12"/>
+      <c r="I25" s="12"/>
+      <c r="J25" s="12"/>
+      <c r="K25" s="12"/>
+    </row>
+    <row r="26" s="107" customFormat="true" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="105" t="s">
         <v>107</v>
       </c>
-      <c r="B25" s="106" t="s">
+      <c r="B26" s="106" t="s">
         <v>40</v>
       </c>
-      <c r="C25" s="106"/>
-      <c r="D25" s="106"/>
-      <c r="E25" s="106"/>
-      <c r="F25" s="106"/>
-      <c r="G25" s="106" t="s">
+      <c r="C26" s="106"/>
+      <c r="D26" s="106"/>
+      <c r="E26" s="106"/>
+      <c r="F26" s="106"/>
+      <c r="G26" s="106" t="s">
         <v>41</v>
       </c>
-      <c r="H25" s="106"/>
-      <c r="I25" s="106" t="s">
+      <c r="H26" s="106"/>
+      <c r="I26" s="106" t="s">
         <v>42</v>
       </c>
-      <c r="J25" s="106"/>
-      <c r="K25" s="106"/>
-    </row>
-    <row r="26" s="110" customFormat="true" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="38"/>
-      <c r="B26" s="98" t="s">
+      <c r="J26" s="106"/>
+      <c r="K26" s="106"/>
+    </row>
+    <row r="27" s="110" customFormat="true" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="38"/>
+      <c r="B27" s="98" t="s">
         <v>108</v>
       </c>
-      <c r="C26" s="108" t="s">
+      <c r="C27" s="108" t="s">
         <v>109</v>
       </c>
-      <c r="D26" s="98" t="s">
+      <c r="D27" s="98" t="s">
         <v>110</v>
       </c>
-      <c r="E26" s="98" t="s">
+      <c r="E27" s="98" t="s">
         <v>111</v>
       </c>
-      <c r="F26" s="98" t="s">
+      <c r="F27" s="98" t="s">
         <v>112</v>
       </c>
-      <c r="G26" s="98" t="s">
+      <c r="G27" s="98" t="s">
         <v>113</v>
       </c>
-      <c r="H26" s="98" t="s">
+      <c r="H27" s="98" t="s">
         <v>114</v>
       </c>
-      <c r="I26" s="98" t="s">
+      <c r="I27" s="98" t="s">
         <v>115</v>
       </c>
-      <c r="J26" s="98" t="s">
+      <c r="J27" s="98" t="s">
         <v>116</v>
       </c>
-      <c r="K26" s="98" t="s">
+      <c r="K27" s="98" t="s">
         <v>117</v>
       </c>
-      <c r="L26" s="109"/>
-      <c r="N26" s="111"/>
-      <c r="O26" s="111"/>
-      <c r="Q26" s="111"/>
-      <c r="R26" s="111"/>
-      <c r="S26" s="109"/>
-      <c r="U26" s="109"/>
-      <c r="V26" s="109"/>
-      <c r="W26" s="109"/>
-      <c r="X26" s="109"/>
-      <c r="Y26" s="109"/>
-    </row>
-    <row r="27" s="20" customFormat="true" ht="51.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="112"/>
-      <c r="B27" s="87"/>
-      <c r="C27" s="87"/>
-      <c r="D27" s="87"/>
-      <c r="E27" s="87"/>
-      <c r="F27" s="87"/>
-      <c r="G27" s="87"/>
-      <c r="H27" s="87"/>
-      <c r="I27" s="87"/>
-      <c r="J27" s="87"/>
-      <c r="K27" s="87"/>
-    </row>
-    <row r="28" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="100" t="s">
+      <c r="L27" s="109"/>
+      <c r="N27" s="111"/>
+      <c r="O27" s="111"/>
+      <c r="Q27" s="111"/>
+      <c r="R27" s="111"/>
+      <c r="S27" s="109"/>
+      <c r="U27" s="109"/>
+      <c r="V27" s="109"/>
+      <c r="W27" s="109"/>
+      <c r="X27" s="109"/>
+      <c r="Y27" s="109"/>
+    </row>
+    <row r="28" s="20" customFormat="true" ht="51.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A28" s="112"/>
+      <c r="B28" s="87"/>
+      <c r="C28" s="87"/>
+      <c r="D28" s="87"/>
+      <c r="E28" s="87"/>
+      <c r="F28" s="87"/>
+      <c r="G28" s="87"/>
+      <c r="H28" s="87"/>
+      <c r="I28" s="87"/>
+      <c r="J28" s="87"/>
+      <c r="K28" s="87"/>
+    </row>
+    <row r="29" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A29" s="100" t="s">
         <v>118</v>
       </c>
-      <c r="B28" s="100"/>
-      <c r="C28" s="100"/>
-      <c r="D28" s="100"/>
-      <c r="E28" s="100"/>
-      <c r="F28" s="100"/>
-      <c r="G28" s="100"/>
-      <c r="H28" s="100"/>
-      <c r="I28" s="100"/>
-      <c r="J28" s="101"/>
-      <c r="K28" s="101"/>
-      <c r="M28" s="113"/>
-    </row>
-    <row r="30" s="40" customFormat="true" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="12" t="s">
+      <c r="B29" s="100"/>
+      <c r="C29" s="100"/>
+      <c r="D29" s="100"/>
+      <c r="E29" s="100"/>
+      <c r="F29" s="100"/>
+      <c r="G29" s="100"/>
+      <c r="H29" s="100"/>
+      <c r="I29" s="100"/>
+      <c r="J29" s="101"/>
+      <c r="K29" s="101"/>
+      <c r="M29" s="113"/>
+    </row>
+    <row r="31" s="40" customFormat="true" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A31" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="B30" s="12"/>
-      <c r="C30" s="12"/>
-      <c r="D30" s="12"/>
-      <c r="E30" s="12"/>
-      <c r="F30" s="12"/>
-      <c r="G30" s="12"/>
-      <c r="H30" s="12"/>
-      <c r="I30" s="12"/>
-      <c r="J30" s="12"/>
-      <c r="K30" s="12"/>
-    </row>
-    <row r="31" s="107" customFormat="true" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="105" t="s">
+      <c r="B31" s="12"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="12"/>
+      <c r="G31" s="12"/>
+      <c r="H31" s="12"/>
+      <c r="I31" s="12"/>
+      <c r="J31" s="12"/>
+      <c r="K31" s="12"/>
+    </row>
+    <row r="32" s="107" customFormat="true" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A32" s="105" t="s">
         <v>120</v>
       </c>
-      <c r="B31" s="106" t="s">
+      <c r="B32" s="106" t="s">
         <v>40</v>
       </c>
-      <c r="C31" s="106"/>
-      <c r="D31" s="106"/>
-      <c r="E31" s="106"/>
-      <c r="F31" s="106"/>
-      <c r="G31" s="106" t="s">
+      <c r="C32" s="106"/>
+      <c r="D32" s="106"/>
+      <c r="E32" s="106"/>
+      <c r="F32" s="106"/>
+      <c r="G32" s="106" t="s">
         <v>41</v>
       </c>
-      <c r="H31" s="106"/>
-      <c r="I31" s="106" t="s">
+      <c r="H32" s="106"/>
+      <c r="I32" s="106" t="s">
         <v>42</v>
       </c>
-      <c r="J31" s="106"/>
-      <c r="K31" s="106"/>
-    </row>
-    <row r="32" s="110" customFormat="true" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="114"/>
-      <c r="B32" s="98" t="s">
+      <c r="J32" s="106"/>
+      <c r="K32" s="106"/>
+    </row>
+    <row r="33" s="110" customFormat="true" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A33" s="114"/>
+      <c r="B33" s="98" t="s">
         <v>121</v>
       </c>
-      <c r="C32" s="108" t="s">
+      <c r="C33" s="108" t="s">
         <v>122</v>
       </c>
-      <c r="D32" s="98" t="s">
+      <c r="D33" s="98" t="s">
         <v>123</v>
       </c>
-      <c r="E32" s="98" t="s">
+      <c r="E33" s="98" t="s">
         <v>124</v>
       </c>
-      <c r="F32" s="98" t="s">
+      <c r="F33" s="98" t="s">
         <v>125</v>
       </c>
-      <c r="G32" s="98" t="s">
+      <c r="G33" s="98" t="s">
         <v>126</v>
       </c>
-      <c r="H32" s="98" t="s">
+      <c r="H33" s="98" t="s">
         <v>127</v>
       </c>
-      <c r="I32" s="98" t="s">
+      <c r="I33" s="98" t="s">
         <v>128</v>
       </c>
-      <c r="J32" s="98" t="s">
+      <c r="J33" s="98" t="s">
         <v>129</v>
       </c>
-      <c r="K32" s="98" t="s">
+      <c r="K33" s="98" t="s">
         <v>130</v>
       </c>
-      <c r="L32" s="109"/>
-      <c r="N32" s="111"/>
-      <c r="O32" s="111"/>
-      <c r="Q32" s="111"/>
-      <c r="R32" s="111"/>
-      <c r="S32" s="109"/>
-      <c r="U32" s="109"/>
-      <c r="V32" s="109"/>
-      <c r="W32" s="109"/>
-      <c r="X32" s="109"/>
-      <c r="Y32" s="109"/>
-    </row>
-    <row r="33" s="20" customFormat="true" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="115"/>
-      <c r="B33" s="87"/>
-      <c r="C33" s="87"/>
-      <c r="D33" s="87"/>
-      <c r="E33" s="87"/>
-      <c r="F33" s="87"/>
-      <c r="G33" s="87"/>
-      <c r="H33" s="87"/>
-      <c r="I33" s="87"/>
-      <c r="J33" s="87"/>
-      <c r="K33" s="87"/>
-    </row>
-    <row r="34" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="100" t="s">
+      <c r="L33" s="109"/>
+      <c r="N33" s="111"/>
+      <c r="O33" s="111"/>
+      <c r="Q33" s="111"/>
+      <c r="R33" s="111"/>
+      <c r="S33" s="109"/>
+      <c r="U33" s="109"/>
+      <c r="V33" s="109"/>
+      <c r="W33" s="109"/>
+      <c r="X33" s="109"/>
+      <c r="Y33" s="109"/>
+    </row>
+    <row r="34" s="20" customFormat="true" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A34" s="115"/>
+      <c r="B34" s="87"/>
+      <c r="C34" s="87"/>
+      <c r="D34" s="87"/>
+      <c r="E34" s="87"/>
+      <c r="F34" s="87"/>
+      <c r="G34" s="87"/>
+      <c r="H34" s="87"/>
+      <c r="I34" s="87"/>
+      <c r="J34" s="87"/>
+      <c r="K34" s="87"/>
+    </row>
+    <row r="35" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A35" s="100" t="s">
         <v>131</v>
       </c>
-      <c r="B34" s="100"/>
-      <c r="C34" s="100"/>
-      <c r="D34" s="100"/>
-      <c r="E34" s="100"/>
-      <c r="F34" s="100"/>
-      <c r="G34" s="100"/>
-      <c r="H34" s="100"/>
-      <c r="I34" s="100"/>
-      <c r="J34" s="101"/>
-      <c r="K34" s="101"/>
-      <c r="M34" s="113"/>
-    </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="65"/>
-      <c r="B35" s="104"/>
-      <c r="C35" s="104"/>
-      <c r="D35" s="104"/>
-      <c r="E35" s="104"/>
-      <c r="F35" s="104"/>
-      <c r="G35" s="104"/>
-      <c r="H35" s="104"/>
-      <c r="I35" s="104"/>
-      <c r="J35" s="104"/>
-      <c r="K35" s="116"/>
-    </row>
-    <row r="36" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="12" t="s">
+      <c r="B35" s="100"/>
+      <c r="C35" s="100"/>
+      <c r="D35" s="100"/>
+      <c r="E35" s="100"/>
+      <c r="F35" s="100"/>
+      <c r="G35" s="100"/>
+      <c r="H35" s="100"/>
+      <c r="I35" s="100"/>
+      <c r="J35" s="101"/>
+      <c r="K35" s="101"/>
+      <c r="M35" s="113"/>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="65"/>
+      <c r="B36" s="104"/>
+      <c r="C36" s="104"/>
+      <c r="D36" s="104"/>
+      <c r="E36" s="104"/>
+      <c r="F36" s="104"/>
+      <c r="G36" s="104"/>
+      <c r="H36" s="104"/>
+      <c r="I36" s="104"/>
+      <c r="J36" s="104"/>
+      <c r="K36" s="116"/>
+    </row>
+    <row r="37" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A37" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="B36" s="12"/>
-      <c r="C36" s="12"/>
-      <c r="D36" s="12"/>
-      <c r="E36" s="12"/>
-      <c r="F36" s="12"/>
-      <c r="G36" s="12"/>
-      <c r="H36" s="12"/>
-      <c r="I36" s="12"/>
-      <c r="J36" s="12"/>
-      <c r="K36" s="12"/>
-    </row>
-    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="113"/>
-      <c r="B37" s="7"/>
-      <c r="C37" s="7"/>
+      <c r="B37" s="12"/>
+      <c r="C37" s="12"/>
+      <c r="D37" s="12"/>
+      <c r="E37" s="12"/>
+      <c r="F37" s="12"/>
+      <c r="G37" s="12"/>
+      <c r="H37" s="12"/>
+      <c r="I37" s="12"/>
+      <c r="J37" s="12"/>
+      <c r="K37" s="12"/>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="113"/>
@@ -3678,93 +3687,97 @@
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="113"/>
-    </row>
-    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="12" t="s">
+      <c r="B39" s="7"/>
+      <c r="C39" s="7"/>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="113"/>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="B41" s="12"/>
-      <c r="C41" s="12"/>
-      <c r="D41" s="12"/>
-      <c r="E41" s="12"/>
-      <c r="F41" s="12"/>
-      <c r="G41" s="12"/>
-      <c r="H41" s="12"/>
-      <c r="I41" s="12"/>
-      <c r="J41" s="12"/>
-      <c r="K41" s="12"/>
-    </row>
-    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="B42" s="7"/>
-      <c r="C42" s="7"/>
-      <c r="D42" s="7"/>
-      <c r="E42" s="7"/>
-      <c r="F42" s="7"/>
-      <c r="G42" s="7"/>
-      <c r="H42" s="7"/>
-      <c r="I42" s="7"/>
-      <c r="J42" s="7"/>
-      <c r="K42" s="7"/>
+      <c r="B42" s="12"/>
+      <c r="C42" s="12"/>
+      <c r="D42" s="12"/>
+      <c r="E42" s="12"/>
+      <c r="F42" s="12"/>
+      <c r="G42" s="12"/>
+      <c r="H42" s="12"/>
+      <c r="I42" s="12"/>
+      <c r="J42" s="12"/>
+      <c r="K42" s="12"/>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B43" s="7"/>
+      <c r="C43" s="7"/>
+      <c r="D43" s="7"/>
+      <c r="E43" s="7"/>
+      <c r="F43" s="7"/>
+      <c r="G43" s="7"/>
+      <c r="H43" s="7"/>
+      <c r="I43" s="7"/>
+      <c r="J43" s="7"/>
+      <c r="K43" s="7"/>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="7" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="27" t="s">
+    <row r="46" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A46" s="27" t="s">
         <v>132</v>
       </c>
-      <c r="B45" s="27"/>
-      <c r="C45" s="27"/>
-      <c r="D45" s="27"/>
-      <c r="E45" s="27"/>
-      <c r="F45" s="27"/>
-      <c r="G45" s="79" t="s">
+      <c r="B46" s="27"/>
+      <c r="C46" s="27"/>
+      <c r="D46" s="27"/>
+      <c r="E46" s="27"/>
+      <c r="F46" s="27"/>
+      <c r="G46" s="79" t="s">
         <v>133</v>
       </c>
-      <c r="H45" s="79"/>
-      <c r="I45" s="79"/>
-      <c r="J45" s="79"/>
-      <c r="K45" s="79"/>
-    </row>
-    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="39"/>
-      <c r="B46" s="39"/>
-      <c r="C46" s="39"/>
-      <c r="D46" s="39"/>
-      <c r="E46" s="39"/>
-      <c r="F46" s="39"/>
-      <c r="G46" s="80"/>
-      <c r="H46" s="80"/>
-      <c r="I46" s="80"/>
-      <c r="J46" s="80"/>
-      <c r="K46" s="80"/>
+      <c r="H46" s="79"/>
+      <c r="I46" s="79"/>
+      <c r="J46" s="79"/>
+      <c r="K46" s="79"/>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="7"/>
-      <c r="B47" s="7"/>
-      <c r="C47" s="7"/>
-      <c r="D47" s="7"/>
-      <c r="E47" s="7"/>
-      <c r="F47" s="7"/>
-      <c r="G47" s="7"/>
-      <c r="H47" s="7"/>
-      <c r="I47" s="7"/>
-      <c r="J47" s="7"/>
-      <c r="K47" s="7"/>
-    </row>
-    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="117"/>
-    </row>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="A47" s="39"/>
+      <c r="B47" s="39"/>
+      <c r="C47" s="39"/>
+      <c r="D47" s="39"/>
+      <c r="E47" s="39"/>
+      <c r="F47" s="39"/>
+      <c r="G47" s="80"/>
+      <c r="H47" s="80"/>
+      <c r="I47" s="80"/>
+      <c r="J47" s="80"/>
+      <c r="K47" s="80"/>
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="7"/>
+      <c r="B48" s="7"/>
+      <c r="C48" s="7"/>
+      <c r="D48" s="7"/>
+      <c r="E48" s="7"/>
+      <c r="F48" s="7"/>
+      <c r="G48" s="7"/>
+      <c r="H48" s="7"/>
+      <c r="I48" s="7"/>
+      <c r="J48" s="7"/>
+      <c r="K48" s="7"/>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="117"/>
+    </row>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="57">
+  <mergeCells count="60">
     <mergeCell ref="G2:J2"/>
     <mergeCell ref="G3:J3"/>
     <mergeCell ref="H5:I5"/>
@@ -3786,42 +3799,45 @@
     <mergeCell ref="G15:H15"/>
     <mergeCell ref="I15:K15"/>
     <mergeCell ref="A16:B16"/>
-    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="F16:F18"/>
     <mergeCell ref="G16:H16"/>
     <mergeCell ref="I16:J16"/>
-    <mergeCell ref="K16:K17"/>
+    <mergeCell ref="K16:K18"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="G17:H17"/>
     <mergeCell ref="I17:J17"/>
-    <mergeCell ref="A19:K19"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="E20:G20"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="A20:K20"/>
     <mergeCell ref="B21:D21"/>
     <mergeCell ref="E21:G21"/>
     <mergeCell ref="H21:I21"/>
     <mergeCell ref="J21:K21"/>
-    <mergeCell ref="A22:I22"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="H22:I22"/>
     <mergeCell ref="J22:K22"/>
-    <mergeCell ref="A24:K24"/>
-    <mergeCell ref="B25:F25"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="I25:K25"/>
-    <mergeCell ref="A28:I28"/>
-    <mergeCell ref="J28:K28"/>
-    <mergeCell ref="A30:K30"/>
-    <mergeCell ref="B31:F31"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="I31:K31"/>
-    <mergeCell ref="A34:I34"/>
-    <mergeCell ref="J34:K34"/>
-    <mergeCell ref="A36:K36"/>
-    <mergeCell ref="A41:K41"/>
-    <mergeCell ref="A45:F45"/>
-    <mergeCell ref="G45:K45"/>
+    <mergeCell ref="A23:I23"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="A25:K25"/>
+    <mergeCell ref="B26:F26"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="I26:K26"/>
+    <mergeCell ref="A29:I29"/>
+    <mergeCell ref="J29:K29"/>
+    <mergeCell ref="A31:K31"/>
+    <mergeCell ref="B32:F32"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="I32:K32"/>
+    <mergeCell ref="A35:I35"/>
+    <mergeCell ref="J35:K35"/>
+    <mergeCell ref="A37:K37"/>
+    <mergeCell ref="A42:K42"/>
     <mergeCell ref="A46:F46"/>
     <mergeCell ref="G46:K46"/>
+    <mergeCell ref="A47:F47"/>
+    <mergeCell ref="G47:K47"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Inclusao data geraçao do documento do demonstrativo financeiro
</commit_message>
<xml_diff>
--- a/sme_ptrf_apps/static/cargas/modelo_demonstrativo_financeiro.xlsx
+++ b/sme_ptrf_apps/static/cargas/modelo_demonstrativo_financeiro.xlsx
@@ -1913,9 +1913,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>54000</xdr:colOff>
+      <xdr:colOff>53640</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>124200</xdr:rowOff>
+      <xdr:rowOff>123840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1929,7 +1929,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="66600" y="152280"/>
-          <a:ext cx="634320" cy="533880"/>
+          <a:ext cx="633960" cy="533520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1955,9 +1955,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>54000</xdr:colOff>
+      <xdr:colOff>53640</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>133560</xdr:rowOff>
+      <xdr:rowOff>133200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1971,7 +1971,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="66600" y="152280"/>
-          <a:ext cx="634320" cy="543240"/>
+          <a:ext cx="633960" cy="542880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3121,8 +3121,8 @@
   </sheetPr>
   <dimension ref="A1:Y1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A27" activeCellId="0" sqref="A27"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A49" activeCellId="0" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3777,7 +3777,7 @@
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="60">
+  <mergeCells count="61">
     <mergeCell ref="G2:J2"/>
     <mergeCell ref="G3:J3"/>
     <mergeCell ref="H5:I5"/>
@@ -3838,6 +3838,7 @@
     <mergeCell ref="G46:K46"/>
     <mergeCell ref="A47:F47"/>
     <mergeCell ref="G47:K47"/>
+    <mergeCell ref="A49:K49"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Modificaçoes no demonstrativo financeiro.
</commit_message>
<xml_diff>
--- a/sme_ptrf_apps/static/cargas/modelo_demonstrativo_financeiro.xlsx
+++ b/sme_ptrf_apps/static/cargas/modelo_demonstrativo_financeiro.xlsx
@@ -217,7 +217,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="150">
   <si>
     <t xml:space="preserve">Prefeitura do Município de São Paulo</t>
   </si>
@@ -795,10 +795,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Demonstrativo Financeiro</t>
-  </si>
-  <si>
-    <t xml:space="preserve">06 - Código EOL da UE</t>
+    <t xml:space="preserve">Demonstrativo Financeiro - FINAL</t>
   </si>
   <si>
     <t xml:space="preserve">08 - Saldo reprogramado do período anterior</t>
@@ -816,7 +813,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">11 - Saldo reprogramado para o próximo período
+      <t xml:space="preserve">12 - Saldo reprogramado para o próximo período
 </t>
     </r>
     <r>
@@ -828,7 +825,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">(08+09-10)</t>
+      <t xml:space="preserve">(08+09-10-11)</t>
     </r>
   </si>
   <si>
@@ -843,7 +840,8 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">09 - Crédito no período </t>
+      <t xml:space="preserve">09 - Créditos
+</t>
     </r>
     <r>
       <rPr>
@@ -854,7 +852,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">(Campo 19 - Bloco 3)</t>
+      <t xml:space="preserve">(Campo 20 - Bloco 3)</t>
     </r>
   </si>
   <si>
@@ -866,7 +864,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">10 - Despesa efetuada no período
+      <t xml:space="preserve">10 - Despesas demonstradas
 </t>
     </r>
     <r>
@@ -878,7 +876,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">(Campo 31 - Bloco 4)</t>
+      <t xml:space="preserve">(Campo 32 - Bloco 4)</t>
     </r>
   </si>
   <si>
@@ -890,7 +888,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">12 - Despesa não demonstrada no extrato do período 
+      <t xml:space="preserve">11 - Despesas não demonstradas
 </t>
     </r>
     <r>
@@ -914,7 +912,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">13 - Saldo bancário ao final do período
+      <t xml:space="preserve">13 - Despesas de períodos anteriores não demonstradas
 </t>
     </r>
     <r>
@@ -926,110 +924,179 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">(11+12)</t>
+      <t xml:space="preserve">(Campo 55 - Bloco 6)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">14 - Saldo bancário ao final do período
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">(12+11+13)</t>
     </r>
   </si>
   <si>
     <t xml:space="preserve">Total </t>
   </si>
   <si>
-    <t xml:space="preserve">BLOCO 3 - CRÉDITOS NO PERÍODO </t>
-  </si>
-  <si>
-    <t xml:space="preserve">14 – Item</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15 – Tipo de Crédito</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16 – Detalhamento</t>
-  </si>
-  <si>
-    <t xml:space="preserve">17 – Data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18 – Valor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">19 – TOTAL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BLOCO 4 - DESPESAS EFETUADAS NO PERÍODO </t>
-  </si>
-  <si>
-    <t xml:space="preserve">20 – Item</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21 – Razão social</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22 - CNPJ ou CPF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">23 - Tipo do documento</t>
-  </si>
-  <si>
-    <t xml:space="preserve">24 - Nº do documento</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25 – Data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">26 – Especificação do material ou serviço</t>
-  </si>
-  <si>
-    <t xml:space="preserve">27 - Tipo da despesa </t>
-  </si>
-  <si>
-    <t xml:space="preserve">28 -  Tipo de transação</t>
-  </si>
-  <si>
-    <t xml:space="preserve">29 - Data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">30 - Valor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">31 – TOTAL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BLOCO 5 - DESPESAS EFETUADAS E NÃO DEMONSTRADAS NO EXTRATO DO PERÍODO (ATUAL E ANTERIORES)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">32 – Item</t>
-  </si>
-  <si>
-    <t xml:space="preserve">33 – Razão social</t>
-  </si>
-  <si>
-    <t xml:space="preserve">34 - CNPJ ou CPF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">35 - Tipo do documento</t>
-  </si>
-  <si>
-    <t xml:space="preserve">36 - Nº do documento</t>
-  </si>
-  <si>
-    <t xml:space="preserve">37 – Data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">38 – Especificação do material ou serviço</t>
-  </si>
-  <si>
-    <t xml:space="preserve">39 - Tipo da despesa </t>
-  </si>
-  <si>
-    <t xml:space="preserve">40 -  Tipo de transação</t>
-  </si>
-  <si>
-    <t xml:space="preserve">41 - Data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">42 - Valor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">43 – TOTAL</t>
+    <t xml:space="preserve">BLOCO 3 - CRÉDITOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15 – Item</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16 – Tipo de Crédito</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17 – Detalhamento</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18 – Data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19 – Valor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20 - TOTAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BLOCO 4 – DESPESAS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21 – Item</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22 – Razão social</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23 - CNPJ ou CPF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24 - Tipo do documento</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25 - Nº do documento</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26 – Data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27 – Especificação do material ou serviço</t>
+  </si>
+  <si>
+    <t xml:space="preserve">28 - Tipo da despesa </t>
+  </si>
+  <si>
+    <t xml:space="preserve">29 -  Tipo de transação</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30 - Data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">31 – Valor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">32 – TOTAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BLOCO 5 - DESPESAS NÃO DEMONSTRADAS NO EXTRATO / DEMONSTRATIVO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">33 – Item</t>
+  </si>
+  <si>
+    <t xml:space="preserve">34 – Razão social</t>
+  </si>
+  <si>
+    <t xml:space="preserve">35 - CNPJ ou CPF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">36 - Tipo do documento</t>
+  </si>
+  <si>
+    <t xml:space="preserve">37 - Nº do documento</t>
+  </si>
+  <si>
+    <t xml:space="preserve">38 – Data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">39 – Especificação do material ou serviço</t>
+  </si>
+  <si>
+    <t xml:space="preserve">40 - Tipo da despesa </t>
+  </si>
+  <si>
+    <t xml:space="preserve">41 -  Tipo de transação</t>
+  </si>
+  <si>
+    <t xml:space="preserve">42 - Data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">43 - Valor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">44 – TOTAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BLOCO 6 - DESPESAS DE PERÍODOS ANTERIORES NÃO DEMONSTRADAS NO EXTRATO / DEMONSTRATIVO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">45 – Item</t>
+  </si>
+  <si>
+    <t xml:space="preserve">46 – Razão social</t>
+  </si>
+  <si>
+    <t xml:space="preserve">47 - CNPJ ou CPF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">48 - Tipo do documento</t>
+  </si>
+  <si>
+    <t xml:space="preserve">49 - Nº do documento</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50 – Data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">51 – Especificação do material ou serviço</t>
+  </si>
+  <si>
+    <t xml:space="preserve">52 - Tipo da despesa </t>
+  </si>
+  <si>
+    <t xml:space="preserve">53 -  Tipo de transação</t>
+  </si>
+  <si>
+    <t xml:space="preserve">54 - Data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">55 - Valor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">56 – TOTAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BLOCO 7 - OBSERVAÇÃO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BLOCO 8 - ASSINATURA DOS RESPONSÁVEIS PELA PRESTAÇÃO DE CONTAS</t>
   </si>
   <si>
     <t xml:space="preserve">______________________________________________
@@ -1038,6 +1105,9 @@
   <si>
     <t xml:space="preserve">___________________________________________
 Assinatura do Presidente do Conselho Fiscal da ASSOCIAÇÃO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Documento final gerado em: DD/MM/AAAA</t>
   </si>
 </sst>
 </file>
@@ -1216,7 +1286,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -1304,6 +1374,13 @@
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="thin"/>
       <top/>
       <bottom/>
       <diagonal/>
@@ -1352,7 +1429,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="118">
+  <cellXfs count="123">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1362,7 +1439,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="15" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -1374,7 +1451,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="15" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -1386,7 +1463,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="15" shrinkToFit="false"/>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1681,10 +1758,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1694,10 +1767,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1705,54 +1774,90 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1781,43 +1886,35 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="21" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="21" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="true"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="21" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="true"/>
-    </xf>
     <xf numFmtId="164" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="21" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="true"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="true"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1913,9 +2010,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>53640</xdr:colOff>
+      <xdr:colOff>63000</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>123840</xdr:rowOff>
+      <xdr:rowOff>133200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1929,7 +2026,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="66600" y="152280"/>
-          <a:ext cx="633960" cy="533520"/>
+          <a:ext cx="643320" cy="542880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1955,9 +2052,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>53640</xdr:colOff>
+      <xdr:colOff>63000</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>133200</xdr:rowOff>
+      <xdr:rowOff>148320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1971,7 +2068,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="66600" y="152280"/>
-          <a:ext cx="633960" cy="542880"/>
+          <a:ext cx="643320" cy="552240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3119,10 +3216,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Y1048576"/>
+  <dimension ref="A1:N1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A49" activeCellId="0" sqref="A49"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G66" activeCellId="0" sqref="G66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3133,8 +3230,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="18.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="16.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="22.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="14.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="23.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="19.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="13.85"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="11.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="15"/>
@@ -3155,7 +3252,7 @@
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
     </row>
-    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
@@ -3176,28 +3273,28 @@
       <c r="D4" s="6"/>
     </row>
     <row r="5" s="7" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="H5" s="82" t="s">
+      <c r="H5" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="82"/>
-      <c r="J5" s="83"/>
-      <c r="K5" s="83"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="82"/>
+      <c r="K5" s="82"/>
     </row>
     <row r="6" s="7" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="H6" s="82" t="s">
+      <c r="H6" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="I6" s="82"/>
-      <c r="J6" s="84"/>
-      <c r="K6" s="84"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="82"/>
+      <c r="K6" s="82"/>
     </row>
     <row r="7" s="7" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="H7" s="82" t="s">
+      <c r="H7" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="I7" s="82"/>
-      <c r="J7" s="85"/>
-      <c r="K7" s="85"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="83"/>
+      <c r="K7" s="83"/>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="9" s="7" customFormat="true" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3227,8 +3324,8 @@
       <c r="G10" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="H10" s="31" t="s">
-        <v>89</v>
+      <c r="H10" s="14" t="s">
+        <v>12</v>
       </c>
       <c r="I10" s="15" t="s">
         <v>13</v>
@@ -3237,20 +3334,33 @@
       <c r="K10" s="15"/>
     </row>
     <row r="11" s="20" customFormat="true" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="86"/>
-      <c r="B11" s="86"/>
-      <c r="C11" s="86"/>
-      <c r="D11" s="86"/>
-      <c r="E11" s="86"/>
-      <c r="F11" s="86"/>
-      <c r="G11" s="87"/>
-      <c r="H11" s="87"/>
-      <c r="I11" s="86"/>
-      <c r="J11" s="86"/>
-      <c r="K11" s="86"/>
-    </row>
-    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="13" s="40" customFormat="true" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="84"/>
+      <c r="B11" s="84"/>
+      <c r="C11" s="84"/>
+      <c r="D11" s="84"/>
+      <c r="E11" s="84"/>
+      <c r="F11" s="84"/>
+      <c r="G11" s="85"/>
+      <c r="H11" s="85"/>
+      <c r="I11" s="84"/>
+      <c r="J11" s="84"/>
+      <c r="K11" s="84"/>
+    </row>
+    <row r="12" s="7" customFormat="true" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="86"/>
+      <c r="B12" s="86"/>
+      <c r="C12" s="86"/>
+      <c r="D12" s="87"/>
+      <c r="E12" s="86"/>
+      <c r="F12" s="88"/>
+      <c r="G12" s="87"/>
+      <c r="H12" s="86"/>
+      <c r="I12" s="86"/>
+      <c r="J12" s="86"/>
+      <c r="K12" s="88"/>
+      <c r="L12" s="89"/>
+    </row>
+    <row r="13" s="7" customFormat="true" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="12" t="s">
         <v>15</v>
       </c>
@@ -3264,98 +3374,104 @@
       <c r="I13" s="12"/>
       <c r="J13" s="12"/>
       <c r="K13" s="12"/>
-    </row>
-    <row r="14" s="7" customFormat="true" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="88" t="s">
+      <c r="L13" s="89"/>
+    </row>
+    <row r="14" s="7" customFormat="true" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="90" t="s">
+        <v>89</v>
+      </c>
+      <c r="B14" s="90"/>
+      <c r="C14" s="91" t="s">
         <v>90</v>
       </c>
-      <c r="B14" s="88"/>
-      <c r="C14" s="88" t="s">
+      <c r="D14" s="91"/>
+      <c r="E14" s="91"/>
+      <c r="F14" s="90" t="s">
         <v>91</v>
       </c>
-      <c r="D14" s="88"/>
-      <c r="E14" s="88" t="s">
+      <c r="G14" s="90"/>
+      <c r="H14" s="92" t="s">
         <v>92</v>
       </c>
-      <c r="F14" s="88"/>
-      <c r="G14" s="88" t="s">
+      <c r="I14" s="92"/>
+      <c r="J14" s="92"/>
+      <c r="K14" s="92"/>
+      <c r="L14" s="89"/>
+    </row>
+    <row r="15" s="7" customFormat="true" ht="50.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="90"/>
+      <c r="B15" s="90"/>
+      <c r="C15" s="93" t="s">
         <v>93</v>
       </c>
-      <c r="H14" s="88"/>
-      <c r="I14" s="88"/>
-      <c r="J14" s="88"/>
-      <c r="K14" s="88"/>
-    </row>
-    <row r="15" s="7" customFormat="true" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="88"/>
-      <c r="B15" s="88"/>
-      <c r="C15" s="89" t="s">
+      <c r="D15" s="94" t="s">
         <v>94</v>
       </c>
-      <c r="D15" s="90" t="s">
+      <c r="E15" s="95" t="s">
         <v>95</v>
       </c>
-      <c r="E15" s="88"/>
-      <c r="F15" s="88"/>
-      <c r="G15" s="89" t="s">
+      <c r="F15" s="90"/>
+      <c r="G15" s="90"/>
+      <c r="H15" s="95" t="s">
         <v>96</v>
       </c>
-      <c r="H15" s="89"/>
-      <c r="I15" s="89" t="s">
+      <c r="I15" s="93" t="s">
         <v>97</v>
       </c>
-      <c r="J15" s="89"/>
-      <c r="K15" s="89"/>
-      <c r="L15" s="91"/>
+      <c r="J15" s="93"/>
+      <c r="K15" s="93"/>
+      <c r="L15" s="89"/>
     </row>
     <row r="16" s="7" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="92"/>
-      <c r="B16" s="92"/>
-      <c r="C16" s="93"/>
-      <c r="D16" s="93"/>
-      <c r="E16" s="93"/>
-      <c r="F16" s="94" t="s">
+      <c r="A16" s="96"/>
+      <c r="B16" s="96"/>
+      <c r="C16" s="97"/>
+      <c r="D16" s="53"/>
+      <c r="E16" s="53"/>
+      <c r="F16" s="97"/>
+      <c r="G16" s="98" t="s">
         <v>98</v>
       </c>
-      <c r="G16" s="92"/>
-      <c r="H16" s="92"/>
-      <c r="I16" s="92"/>
-      <c r="J16" s="92"/>
-      <c r="K16" s="95" t="s">
+      <c r="H16" s="99"/>
+      <c r="I16" s="97"/>
+      <c r="J16" s="97"/>
+      <c r="K16" s="100" t="s">
         <v>98</v>
       </c>
-      <c r="L16" s="91"/>
+      <c r="L16" s="89"/>
     </row>
     <row r="17" s="7" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="92"/>
-      <c r="B17" s="92"/>
-      <c r="C17" s="93"/>
-      <c r="D17" s="93"/>
-      <c r="E17" s="93"/>
-      <c r="F17" s="94"/>
-      <c r="G17" s="92"/>
-      <c r="H17" s="92"/>
-      <c r="I17" s="92"/>
-      <c r="J17" s="92"/>
-      <c r="K17" s="95"/>
-      <c r="L17" s="91"/>
+      <c r="A17" s="101"/>
+      <c r="B17" s="101"/>
+      <c r="C17" s="102"/>
+      <c r="D17" s="54"/>
+      <c r="E17" s="54"/>
+      <c r="F17" s="102"/>
+      <c r="G17" s="98"/>
+      <c r="H17" s="64"/>
+      <c r="I17" s="102"/>
+      <c r="J17" s="102"/>
+      <c r="K17" s="100"/>
+      <c r="L17" s="89"/>
     </row>
     <row r="18" s="7" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="96"/>
-      <c r="B18" s="96"/>
-      <c r="C18" s="97"/>
-      <c r="D18" s="97"/>
-      <c r="E18" s="97"/>
-      <c r="F18" s="94"/>
-      <c r="G18" s="96"/>
-      <c r="H18" s="96"/>
-      <c r="I18" s="96"/>
-      <c r="J18" s="96"/>
-      <c r="K18" s="95"/>
-      <c r="L18" s="91"/>
-    </row>
-    <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="20" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="103"/>
+      <c r="B18" s="103"/>
+      <c r="C18" s="104"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="104"/>
+      <c r="G18" s="98"/>
+      <c r="H18" s="105"/>
+      <c r="I18" s="104"/>
+      <c r="J18" s="104"/>
+      <c r="K18" s="100"/>
+      <c r="L18" s="89"/>
+    </row>
+    <row r="19" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="M19" s="7"/>
+    </row>
+    <row r="20" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="12" t="s">
         <v>99</v>
       </c>
@@ -3369,72 +3485,75 @@
       <c r="I20" s="12"/>
       <c r="J20" s="12"/>
       <c r="K20" s="12"/>
+      <c r="M20" s="7"/>
     </row>
     <row r="21" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="98" t="s">
+      <c r="A21" s="106" t="s">
         <v>100</v>
       </c>
-      <c r="B21" s="98" t="s">
+      <c r="B21" s="106" t="s">
         <v>101</v>
       </c>
-      <c r="C21" s="98"/>
-      <c r="D21" s="98"/>
-      <c r="E21" s="98" t="s">
+      <c r="C21" s="106"/>
+      <c r="D21" s="106"/>
+      <c r="E21" s="106" t="s">
         <v>102</v>
       </c>
-      <c r="F21" s="98"/>
-      <c r="G21" s="98"/>
-      <c r="H21" s="98" t="s">
+      <c r="F21" s="106"/>
+      <c r="G21" s="106"/>
+      <c r="H21" s="106" t="s">
         <v>103</v>
       </c>
-      <c r="I21" s="98"/>
-      <c r="J21" s="98" t="s">
+      <c r="I21" s="106"/>
+      <c r="J21" s="106" t="s">
         <v>104</v>
       </c>
-      <c r="K21" s="98"/>
+      <c r="K21" s="106"/>
     </row>
     <row r="22" customFormat="false" ht="51.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="86"/>
-      <c r="B22" s="99"/>
-      <c r="C22" s="99"/>
-      <c r="D22" s="99"/>
-      <c r="E22" s="99"/>
-      <c r="F22" s="99"/>
-      <c r="G22" s="99"/>
-      <c r="H22" s="99"/>
-      <c r="I22" s="99"/>
-      <c r="J22" s="99"/>
-      <c r="K22" s="99"/>
-    </row>
-    <row r="23" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="100" t="s">
+      <c r="A22" s="84"/>
+      <c r="B22" s="85"/>
+      <c r="C22" s="85"/>
+      <c r="D22" s="85"/>
+      <c r="E22" s="85"/>
+      <c r="F22" s="85"/>
+      <c r="G22" s="85"/>
+      <c r="H22" s="85"/>
+      <c r="I22" s="85"/>
+      <c r="J22" s="85"/>
+      <c r="K22" s="85"/>
+    </row>
+    <row r="23" customFormat="false" ht="18.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="107" t="s">
         <v>105</v>
       </c>
-      <c r="B23" s="100"/>
-      <c r="C23" s="100"/>
-      <c r="D23" s="100"/>
-      <c r="E23" s="100"/>
-      <c r="F23" s="100"/>
-      <c r="G23" s="100"/>
-      <c r="H23" s="100"/>
-      <c r="I23" s="100"/>
-      <c r="J23" s="101"/>
-      <c r="K23" s="101"/>
+      <c r="B23" s="107"/>
+      <c r="C23" s="107"/>
+      <c r="D23" s="107"/>
+      <c r="E23" s="107"/>
+      <c r="F23" s="107"/>
+      <c r="G23" s="107"/>
+      <c r="H23" s="107"/>
+      <c r="I23" s="107"/>
+      <c r="J23" s="108"/>
+      <c r="K23" s="108"/>
+      <c r="M23" s="7"/>
+      <c r="N23" s="7"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="102"/>
-      <c r="B24" s="103"/>
-      <c r="C24" s="103"/>
-      <c r="D24" s="103"/>
-      <c r="E24" s="103"/>
-      <c r="F24" s="103"/>
-      <c r="G24" s="103"/>
-      <c r="H24" s="104"/>
-      <c r="I24" s="104"/>
-      <c r="J24" s="104"/>
-      <c r="K24" s="104"/>
-    </row>
-    <row r="25" s="40" customFormat="true" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="109"/>
+      <c r="B24" s="110"/>
+      <c r="C24" s="110"/>
+      <c r="D24" s="110"/>
+      <c r="E24" s="110"/>
+      <c r="F24" s="110"/>
+      <c r="G24" s="110"/>
+      <c r="H24" s="111"/>
+      <c r="I24" s="111"/>
+      <c r="J24" s="111"/>
+      <c r="K24" s="111"/>
+    </row>
+    <row r="25" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="12" t="s">
         <v>106</v>
       </c>
@@ -3449,101 +3568,102 @@
       <c r="J25" s="12"/>
       <c r="K25" s="12"/>
     </row>
-    <row r="26" s="107" customFormat="true" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="105" t="s">
+    <row r="26" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="112" t="s">
         <v>107</v>
       </c>
-      <c r="B26" s="106" t="s">
+      <c r="B26" s="113" t="s">
         <v>40</v>
       </c>
-      <c r="C26" s="106"/>
-      <c r="D26" s="106"/>
-      <c r="E26" s="106"/>
-      <c r="F26" s="106"/>
-      <c r="G26" s="106" t="s">
+      <c r="C26" s="113"/>
+      <c r="D26" s="113"/>
+      <c r="E26" s="113"/>
+      <c r="F26" s="113"/>
+      <c r="G26" s="113" t="s">
         <v>41</v>
       </c>
-      <c r="H26" s="106"/>
-      <c r="I26" s="106" t="s">
+      <c r="H26" s="113"/>
+      <c r="I26" s="113" t="s">
         <v>42</v>
       </c>
-      <c r="J26" s="106"/>
-      <c r="K26" s="106"/>
-    </row>
-    <row r="27" s="110" customFormat="true" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="38"/>
-      <c r="B27" s="98" t="s">
+      <c r="J26" s="113"/>
+      <c r="K26" s="113"/>
+    </row>
+    <row r="27" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="114"/>
+      <c r="B27" s="106" t="s">
         <v>108</v>
       </c>
-      <c r="C27" s="108" t="s">
+      <c r="C27" s="115" t="s">
         <v>109</v>
       </c>
-      <c r="D27" s="98" t="s">
+      <c r="D27" s="106" t="s">
         <v>110</v>
       </c>
-      <c r="E27" s="98" t="s">
+      <c r="E27" s="106" t="s">
         <v>111</v>
       </c>
-      <c r="F27" s="98" t="s">
+      <c r="F27" s="106" t="s">
         <v>112</v>
       </c>
-      <c r="G27" s="98" t="s">
+      <c r="G27" s="106" t="s">
         <v>113</v>
       </c>
-      <c r="H27" s="98" t="s">
+      <c r="H27" s="106" t="s">
         <v>114</v>
       </c>
-      <c r="I27" s="98" t="s">
+      <c r="I27" s="106" t="s">
         <v>115</v>
       </c>
-      <c r="J27" s="98" t="s">
+      <c r="J27" s="106" t="s">
         <v>116</v>
       </c>
-      <c r="K27" s="98" t="s">
+      <c r="K27" s="106" t="s">
         <v>117</v>
       </c>
-      <c r="L27" s="109"/>
-      <c r="N27" s="111"/>
-      <c r="O27" s="111"/>
-      <c r="Q27" s="111"/>
-      <c r="R27" s="111"/>
-      <c r="S27" s="109"/>
-      <c r="U27" s="109"/>
-      <c r="V27" s="109"/>
-      <c r="W27" s="109"/>
-      <c r="X27" s="109"/>
-      <c r="Y27" s="109"/>
-    </row>
-    <row r="28" s="20" customFormat="true" ht="51.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="112"/>
-      <c r="B28" s="87"/>
-      <c r="C28" s="87"/>
-      <c r="D28" s="87"/>
-      <c r="E28" s="87"/>
-      <c r="F28" s="87"/>
-      <c r="G28" s="87"/>
-      <c r="H28" s="87"/>
-      <c r="I28" s="87"/>
-      <c r="J28" s="87"/>
-      <c r="K28" s="87"/>
-    </row>
-    <row r="29" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="100" t="s">
+    </row>
+    <row r="28" s="40" customFormat="true" ht="51.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A28" s="116"/>
+      <c r="B28" s="85"/>
+      <c r="C28" s="85"/>
+      <c r="D28" s="85"/>
+      <c r="E28" s="85"/>
+      <c r="F28" s="85"/>
+      <c r="G28" s="85"/>
+      <c r="H28" s="85"/>
+      <c r="I28" s="85"/>
+      <c r="J28" s="85"/>
+      <c r="K28" s="85"/>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="107" t="s">
         <v>118</v>
       </c>
-      <c r="B29" s="100"/>
-      <c r="C29" s="100"/>
-      <c r="D29" s="100"/>
-      <c r="E29" s="100"/>
-      <c r="F29" s="100"/>
-      <c r="G29" s="100"/>
-      <c r="H29" s="100"/>
-      <c r="I29" s="100"/>
-      <c r="J29" s="101"/>
-      <c r="K29" s="101"/>
-      <c r="M29" s="113"/>
-    </row>
-    <row r="31" s="40" customFormat="true" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B29" s="107"/>
+      <c r="C29" s="107"/>
+      <c r="D29" s="107"/>
+      <c r="E29" s="107"/>
+      <c r="F29" s="107"/>
+      <c r="G29" s="107"/>
+      <c r="H29" s="107"/>
+      <c r="I29" s="107"/>
+      <c r="J29" s="108"/>
+      <c r="K29" s="108"/>
+    </row>
+    <row r="30" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
+      <c r="K30" s="1"/>
+    </row>
+    <row r="31" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="12" t="s">
         <v>119</v>
       </c>
@@ -3558,116 +3678,91 @@
       <c r="J31" s="12"/>
       <c r="K31" s="12"/>
     </row>
-    <row r="32" s="107" customFormat="true" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="105" t="s">
+    <row r="32" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A32" s="112" t="s">
         <v>120</v>
       </c>
-      <c r="B32" s="106" t="s">
+      <c r="B32" s="113" t="s">
         <v>40</v>
       </c>
-      <c r="C32" s="106"/>
-      <c r="D32" s="106"/>
-      <c r="E32" s="106"/>
-      <c r="F32" s="106"/>
-      <c r="G32" s="106" t="s">
+      <c r="C32" s="113"/>
+      <c r="D32" s="113"/>
+      <c r="E32" s="113"/>
+      <c r="F32" s="113"/>
+      <c r="G32" s="113" t="s">
         <v>41</v>
       </c>
-      <c r="H32" s="106"/>
-      <c r="I32" s="106" t="s">
+      <c r="H32" s="113"/>
+      <c r="I32" s="113" t="s">
         <v>42</v>
       </c>
-      <c r="J32" s="106"/>
-      <c r="K32" s="106"/>
-    </row>
-    <row r="33" s="110" customFormat="true" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="114"/>
-      <c r="B33" s="98" t="s">
+      <c r="J32" s="113"/>
+      <c r="K32" s="113"/>
+    </row>
+    <row r="33" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="117"/>
+      <c r="B33" s="106" t="s">
         <v>121</v>
       </c>
-      <c r="C33" s="108" t="s">
+      <c r="C33" s="115" t="s">
         <v>122</v>
       </c>
-      <c r="D33" s="98" t="s">
+      <c r="D33" s="106" t="s">
         <v>123</v>
       </c>
-      <c r="E33" s="98" t="s">
+      <c r="E33" s="106" t="s">
         <v>124</v>
       </c>
-      <c r="F33" s="98" t="s">
+      <c r="F33" s="106" t="s">
         <v>125</v>
       </c>
-      <c r="G33" s="98" t="s">
+      <c r="G33" s="106" t="s">
         <v>126</v>
       </c>
-      <c r="H33" s="98" t="s">
+      <c r="H33" s="106" t="s">
         <v>127</v>
       </c>
-      <c r="I33" s="98" t="s">
+      <c r="I33" s="106" t="s">
         <v>128</v>
       </c>
-      <c r="J33" s="98" t="s">
+      <c r="J33" s="106" t="s">
         <v>129</v>
       </c>
-      <c r="K33" s="98" t="s">
+      <c r="K33" s="106" t="s">
         <v>130</v>
       </c>
-      <c r="L33" s="109"/>
-      <c r="N33" s="111"/>
-      <c r="O33" s="111"/>
-      <c r="Q33" s="111"/>
-      <c r="R33" s="111"/>
-      <c r="S33" s="109"/>
-      <c r="U33" s="109"/>
-      <c r="V33" s="109"/>
-      <c r="W33" s="109"/>
-      <c r="X33" s="109"/>
-      <c r="Y33" s="109"/>
-    </row>
-    <row r="34" s="20" customFormat="true" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="115"/>
-      <c r="B34" s="87"/>
-      <c r="C34" s="87"/>
-      <c r="D34" s="87"/>
-      <c r="E34" s="87"/>
-      <c r="F34" s="87"/>
-      <c r="G34" s="87"/>
-      <c r="H34" s="87"/>
-      <c r="I34" s="87"/>
-      <c r="J34" s="87"/>
-      <c r="K34" s="87"/>
-    </row>
-    <row r="35" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="100" t="s">
+    </row>
+    <row r="34" s="40" customFormat="true" ht="51.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A34" s="118"/>
+      <c r="B34" s="85"/>
+      <c r="C34" s="85"/>
+      <c r="D34" s="85"/>
+      <c r="E34" s="85"/>
+      <c r="F34" s="85"/>
+      <c r="G34" s="85"/>
+      <c r="H34" s="85"/>
+      <c r="I34" s="85"/>
+      <c r="J34" s="85"/>
+      <c r="K34" s="85"/>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="107" t="s">
         <v>131</v>
       </c>
-      <c r="B35" s="100"/>
-      <c r="C35" s="100"/>
-      <c r="D35" s="100"/>
-      <c r="E35" s="100"/>
-      <c r="F35" s="100"/>
-      <c r="G35" s="100"/>
-      <c r="H35" s="100"/>
-      <c r="I35" s="100"/>
-      <c r="J35" s="101"/>
-      <c r="K35" s="101"/>
-      <c r="M35" s="113"/>
-    </row>
-    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="65"/>
-      <c r="B36" s="104"/>
-      <c r="C36" s="104"/>
-      <c r="D36" s="104"/>
-      <c r="E36" s="104"/>
-      <c r="F36" s="104"/>
-      <c r="G36" s="104"/>
-      <c r="H36" s="104"/>
-      <c r="I36" s="104"/>
-      <c r="J36" s="104"/>
-      <c r="K36" s="116"/>
+      <c r="B35" s="107"/>
+      <c r="C35" s="107"/>
+      <c r="D35" s="107"/>
+      <c r="E35" s="107"/>
+      <c r="F35" s="107"/>
+      <c r="G35" s="107"/>
+      <c r="H35" s="107"/>
+      <c r="I35" s="107"/>
+      <c r="J35" s="108"/>
+      <c r="K35" s="108"/>
     </row>
     <row r="37" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="12" t="s">
-        <v>77</v>
+        <v>132</v>
       </c>
       <c r="B37" s="12"/>
       <c r="C37" s="12"/>
@@ -3680,104 +3775,231 @@
       <c r="J37" s="12"/>
       <c r="K37" s="12"/>
     </row>
-    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="113"/>
-      <c r="B38" s="7"/>
-      <c r="C38" s="7"/>
-    </row>
-    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="113"/>
-      <c r="B39" s="7"/>
-      <c r="C39" s="7"/>
-    </row>
-    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="113"/>
+    <row r="38" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A38" s="112" t="s">
+        <v>133</v>
+      </c>
+      <c r="B38" s="113" t="s">
+        <v>40</v>
+      </c>
+      <c r="C38" s="113"/>
+      <c r="D38" s="113"/>
+      <c r="E38" s="113"/>
+      <c r="F38" s="113"/>
+      <c r="G38" s="113" t="s">
+        <v>41</v>
+      </c>
+      <c r="H38" s="113"/>
+      <c r="I38" s="113" t="s">
+        <v>42</v>
+      </c>
+      <c r="J38" s="113"/>
+      <c r="K38" s="113"/>
+    </row>
+    <row r="39" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A39" s="117"/>
+      <c r="B39" s="106" t="s">
+        <v>134</v>
+      </c>
+      <c r="C39" s="115" t="s">
+        <v>135</v>
+      </c>
+      <c r="D39" s="106" t="s">
+        <v>136</v>
+      </c>
+      <c r="E39" s="106" t="s">
+        <v>137</v>
+      </c>
+      <c r="F39" s="106" t="s">
+        <v>138</v>
+      </c>
+      <c r="G39" s="106" t="s">
+        <v>139</v>
+      </c>
+      <c r="H39" s="106" t="s">
+        <v>140</v>
+      </c>
+      <c r="I39" s="106" t="s">
+        <v>141</v>
+      </c>
+      <c r="J39" s="106" t="s">
+        <v>142</v>
+      </c>
+      <c r="K39" s="106" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="40" s="40" customFormat="true" ht="51.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A40" s="118"/>
+      <c r="B40" s="85"/>
+      <c r="C40" s="85"/>
+      <c r="D40" s="85"/>
+      <c r="E40" s="85"/>
+      <c r="F40" s="85"/>
+      <c r="G40" s="85"/>
+      <c r="H40" s="85"/>
+      <c r="I40" s="85"/>
+      <c r="J40" s="85"/>
+      <c r="K40" s="85"/>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="107" t="s">
+        <v>144</v>
+      </c>
+      <c r="B41" s="107"/>
+      <c r="C41" s="107"/>
+      <c r="D41" s="107"/>
+      <c r="E41" s="107"/>
+      <c r="F41" s="107"/>
+      <c r="G41" s="107"/>
+      <c r="H41" s="107"/>
+      <c r="I41" s="107"/>
+      <c r="J41" s="108"/>
+      <c r="K41" s="108"/>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="B42" s="12"/>
-      <c r="C42" s="12"/>
-      <c r="D42" s="12"/>
-      <c r="E42" s="12"/>
-      <c r="F42" s="12"/>
-      <c r="G42" s="12"/>
-      <c r="H42" s="12"/>
-      <c r="I42" s="12"/>
-      <c r="J42" s="12"/>
-      <c r="K42" s="12"/>
+      <c r="A42" s="65"/>
+      <c r="B42" s="111"/>
+      <c r="C42" s="111"/>
+      <c r="D42" s="111"/>
+      <c r="E42" s="111"/>
+      <c r="F42" s="111"/>
+      <c r="G42" s="111"/>
+      <c r="H42" s="111"/>
+      <c r="I42" s="111"/>
+      <c r="J42" s="111"/>
+      <c r="K42" s="119"/>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="7" t="s">
+      <c r="A43" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="B43" s="12"/>
+      <c r="C43" s="12"/>
+      <c r="D43" s="12"/>
+      <c r="E43" s="12"/>
+      <c r="F43" s="12"/>
+      <c r="G43" s="12"/>
+      <c r="H43" s="12"/>
+      <c r="I43" s="12"/>
+      <c r="J43" s="12"/>
+      <c r="K43" s="12"/>
+    </row>
+    <row r="44" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A44" s="120"/>
+      <c r="B44" s="7"/>
+      <c r="C44" s="7"/>
+    </row>
+    <row r="45" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A45" s="120"/>
+      <c r="B45" s="7"/>
+      <c r="C45" s="7"/>
+    </row>
+    <row r="46" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A46" s="120"/>
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="B48" s="12"/>
+      <c r="C48" s="12"/>
+      <c r="D48" s="12"/>
+      <c r="E48" s="12"/>
+      <c r="F48" s="12"/>
+      <c r="G48" s="12"/>
+      <c r="H48" s="12"/>
+      <c r="I48" s="12"/>
+      <c r="J48" s="12"/>
+      <c r="K48" s="12"/>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="B43" s="7"/>
-      <c r="C43" s="7"/>
-      <c r="D43" s="7"/>
-      <c r="E43" s="7"/>
-      <c r="F43" s="7"/>
-      <c r="G43" s="7"/>
-      <c r="H43" s="7"/>
-      <c r="I43" s="7"/>
-      <c r="J43" s="7"/>
-      <c r="K43" s="7"/>
-    </row>
-    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="7" t="s">
+      <c r="B49" s="7"/>
+      <c r="C49" s="7"/>
+      <c r="D49" s="7"/>
+      <c r="E49" s="7"/>
+      <c r="F49" s="7"/>
+      <c r="G49" s="7"/>
+      <c r="H49" s="7"/>
+      <c r="I49" s="7"/>
+      <c r="J49" s="7"/>
+      <c r="K49" s="7"/>
+    </row>
+    <row r="50" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A50" s="7" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A46" s="27" t="s">
-        <v>132</v>
-      </c>
-      <c r="B46" s="27"/>
-      <c r="C46" s="27"/>
-      <c r="D46" s="27"/>
-      <c r="E46" s="27"/>
-      <c r="F46" s="27"/>
-      <c r="G46" s="79" t="s">
-        <v>133</v>
-      </c>
-      <c r="H46" s="79"/>
-      <c r="I46" s="79"/>
-      <c r="J46" s="79"/>
-      <c r="K46" s="79"/>
-    </row>
-    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="39"/>
-      <c r="B47" s="39"/>
-      <c r="C47" s="39"/>
-      <c r="D47" s="39"/>
-      <c r="E47" s="39"/>
-      <c r="F47" s="39"/>
-      <c r="G47" s="80"/>
-      <c r="H47" s="80"/>
-      <c r="I47" s="80"/>
-      <c r="J47" s="80"/>
-      <c r="K47" s="80"/>
-    </row>
-    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="7"/>
-      <c r="B48" s="7"/>
-      <c r="C48" s="7"/>
-      <c r="D48" s="7"/>
-      <c r="E48" s="7"/>
-      <c r="F48" s="7"/>
-      <c r="G48" s="7"/>
-      <c r="H48" s="7"/>
-      <c r="I48" s="7"/>
-      <c r="J48" s="7"/>
-      <c r="K48" s="7"/>
-    </row>
-    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="117"/>
-    </row>
+    <row r="51" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="52" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A52" s="27" t="s">
+        <v>147</v>
+      </c>
+      <c r="B52" s="27"/>
+      <c r="C52" s="27"/>
+      <c r="D52" s="27"/>
+      <c r="E52" s="27"/>
+      <c r="F52" s="27"/>
+      <c r="G52" s="79" t="s">
+        <v>148</v>
+      </c>
+      <c r="H52" s="79"/>
+      <c r="I52" s="79"/>
+      <c r="J52" s="79"/>
+      <c r="K52" s="79"/>
+    </row>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="39"/>
+      <c r="B53" s="39"/>
+      <c r="C53" s="39"/>
+      <c r="D53" s="39"/>
+      <c r="E53" s="39"/>
+      <c r="F53" s="39"/>
+      <c r="G53" s="121"/>
+      <c r="H53" s="121"/>
+      <c r="I53" s="121"/>
+      <c r="J53" s="121"/>
+      <c r="K53" s="121"/>
+    </row>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="7"/>
+      <c r="B54" s="7"/>
+      <c r="C54" s="7"/>
+      <c r="D54" s="7"/>
+      <c r="E54" s="7"/>
+      <c r="F54" s="7"/>
+      <c r="G54" s="7"/>
+      <c r="H54" s="7"/>
+      <c r="I54" s="7"/>
+      <c r="J54" s="7"/>
+      <c r="K54" s="7"/>
+    </row>
+    <row r="55" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="7" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="122"/>
+    </row>
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="122"/>
+    </row>
+    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="61">
+  <mergeCells count="62">
     <mergeCell ref="G2:J2"/>
     <mergeCell ref="G3:J3"/>
     <mergeCell ref="H5:I5"/>
@@ -3793,21 +4015,17 @@
     <mergeCell ref="I11:K11"/>
     <mergeCell ref="A13:K13"/>
     <mergeCell ref="A14:B15"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="E14:F15"/>
-    <mergeCell ref="G14:K14"/>
-    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="F14:G15"/>
+    <mergeCell ref="H14:K14"/>
     <mergeCell ref="I15:K15"/>
     <mergeCell ref="A16:B16"/>
-    <mergeCell ref="F16:F18"/>
-    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="G16:G18"/>
     <mergeCell ref="I16:J16"/>
     <mergeCell ref="K16:K18"/>
     <mergeCell ref="A17:B17"/>
-    <mergeCell ref="G17:H17"/>
     <mergeCell ref="I17:J17"/>
     <mergeCell ref="A18:B18"/>
-    <mergeCell ref="G18:H18"/>
     <mergeCell ref="I18:J18"/>
     <mergeCell ref="A20:K20"/>
     <mergeCell ref="B21:D21"/>
@@ -3833,12 +4051,17 @@
     <mergeCell ref="A35:I35"/>
     <mergeCell ref="J35:K35"/>
     <mergeCell ref="A37:K37"/>
-    <mergeCell ref="A42:K42"/>
-    <mergeCell ref="A46:F46"/>
-    <mergeCell ref="G46:K46"/>
-    <mergeCell ref="A47:F47"/>
-    <mergeCell ref="G47:K47"/>
-    <mergeCell ref="A49:K49"/>
+    <mergeCell ref="B38:F38"/>
+    <mergeCell ref="G38:H38"/>
+    <mergeCell ref="I38:K38"/>
+    <mergeCell ref="A41:I41"/>
+    <mergeCell ref="J41:K41"/>
+    <mergeCell ref="A43:K43"/>
+    <mergeCell ref="A48:K48"/>
+    <mergeCell ref="A52:F52"/>
+    <mergeCell ref="G52:K52"/>
+    <mergeCell ref="A53:F53"/>
+    <mergeCell ref="G53:K53"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>